<commit_message>
comming along.  making all the required plots.  just finished qq
</commit_message>
<xml_diff>
--- a/velocity.xlsx
+++ b/velocity.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,20 +8,34 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Documents\TAMU\Spring_2023\final_proj\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{B2F5A212-4C60-4263-81DD-88F557DCA6B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA72CE8E-7D01-4EA0-92AF-44370854B266}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="velocity" sheetId="1" r:id="rId1"/>
     <sheet name="wide" sheetId="2" r:id="rId2"/>
+    <sheet name="summary table" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="19">
   <si>
     <t>cnt</t>
   </si>
@@ -61,12 +75,33 @@
   <si>
     <t>Velocity (fps)</t>
   </si>
+  <si>
+    <t>Rifle</t>
+  </si>
+  <si>
+    <t>Amo</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>µ</t>
+  </si>
+  <si>
+    <t>σ</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="20" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="#,##0.0"/>
+  </numFmts>
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -211,6 +246,22 @@
     </font>
     <font>
       <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <strike/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -416,7 +467,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -583,6 +634,170 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -628,19 +843,22 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="35" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="35" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="16" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="35" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -650,13 +868,60 @@
     <xf numFmtId="0" fontId="18" fillId="35" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="35" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="18" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="18" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="18" fillId="34" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="18" fillId="34" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="18" fillId="34" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="18" fillId="34" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="35" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="18" fillId="34" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="18" fillId="34" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="18" fillId="34" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="18" fillId="34" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="18" fillId="34" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="18" fillId="34" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="21" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1011,11 +1276,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D109"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2552,18 +2817,18 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:O46"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="M33" sqref="M33"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="Q9" sqref="Q9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11" style="2" customWidth="1"/>
-    <col min="2" max="2" width="11.88671875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="17" style="2" customWidth="1"/>
+    <col min="1" max="1" width="11" customWidth="1"/>
+    <col min="2" max="2" width="11.88671875" customWidth="1"/>
+    <col min="3" max="3" width="17" customWidth="1"/>
     <col min="4" max="4" width="1.6640625" customWidth="1"/>
     <col min="5" max="5" width="11" customWidth="1"/>
     <col min="6" max="6" width="11.88671875" customWidth="1"/>
@@ -2579,953 +2844,953 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="18" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="I1" s="3" t="s">
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="I1" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12"/>
+      <c r="O1" s="12"/>
     </row>
     <row r="2" spans="1:15" ht="18" x14ac:dyDescent="0.35">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="13"/>
-      <c r="E2" s="9" t="s">
+      <c r="D2" s="8"/>
+      <c r="E2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="4"/>
-      <c r="I2" s="9" t="s">
+      <c r="H2" s="2"/>
+      <c r="I2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="9" t="s">
+      <c r="J2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="9" t="s">
+      <c r="K2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="L2" s="10"/>
-      <c r="M2" s="9" t="s">
+      <c r="L2" s="5"/>
+      <c r="M2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="N2" s="9" t="s">
+      <c r="N2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="O2" s="9" t="s">
+      <c r="O2" s="4" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="12" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="1">
         <v>1</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="3">
         <v>2565</v>
       </c>
-      <c r="D3" s="11"/>
-      <c r="E3" s="6" t="s">
+      <c r="D3" s="6"/>
+      <c r="E3" s="9" t="s">
         <v>6</v>
       </c>
       <c r="F3" s="1">
         <v>3</v>
       </c>
-      <c r="G3" s="5">
+      <c r="G3" s="3">
         <v>2441</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="I3" s="9" t="s">
         <v>4</v>
       </c>
       <c r="J3" s="1">
         <v>1</v>
       </c>
-      <c r="K3" s="5">
+      <c r="K3" s="37">
         <v>2393</v>
       </c>
-      <c r="L3" s="11"/>
-      <c r="M3" s="6" t="s">
+      <c r="L3" s="6"/>
+      <c r="M3" s="9" t="s">
         <v>6</v>
       </c>
       <c r="N3" s="1">
         <v>3</v>
       </c>
-      <c r="O3" s="5">
+      <c r="O3" s="3">
         <v>2438</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="3"/>
+      <c r="A4" s="12"/>
       <c r="B4" s="1">
         <v>5</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="3">
         <v>2532</v>
       </c>
-      <c r="D4" s="11"/>
-      <c r="E4" s="7"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="10"/>
       <c r="F4" s="1">
         <v>7</v>
       </c>
-      <c r="G4" s="5">
+      <c r="G4" s="3">
         <v>2436</v>
       </c>
-      <c r="I4" s="7"/>
+      <c r="I4" s="10"/>
       <c r="J4" s="1">
         <v>5</v>
       </c>
-      <c r="K4" s="5">
+      <c r="K4" s="3">
         <v>2550</v>
       </c>
-      <c r="L4" s="11"/>
-      <c r="M4" s="7"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="10"/>
       <c r="N4" s="1">
         <v>7</v>
       </c>
-      <c r="O4" s="5">
+      <c r="O4" s="3">
         <v>2439</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="3"/>
+      <c r="A5" s="12"/>
       <c r="B5" s="1">
         <v>9</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="3">
         <v>2566</v>
       </c>
-      <c r="D5" s="11"/>
-      <c r="E5" s="7"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="10"/>
       <c r="F5" s="1">
         <v>11</v>
       </c>
-      <c r="G5" s="5">
+      <c r="G5" s="3">
         <v>2441</v>
       </c>
-      <c r="I5" s="7"/>
+      <c r="I5" s="10"/>
       <c r="J5" s="1">
         <v>9</v>
       </c>
-      <c r="K5" s="5">
+      <c r="K5" s="3">
         <v>2599</v>
       </c>
-      <c r="L5" s="11"/>
-      <c r="M5" s="7"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="10"/>
       <c r="N5" s="1">
         <v>11</v>
       </c>
-      <c r="O5" s="5">
+      <c r="O5" s="3">
         <v>2460</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="3"/>
+      <c r="A6" s="12"/>
       <c r="B6" s="1">
         <v>13</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="3">
         <v>2586</v>
       </c>
-      <c r="D6" s="11"/>
-      <c r="E6" s="7"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="10"/>
       <c r="F6" s="1">
         <v>15</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G6" s="3">
         <v>2438</v>
       </c>
-      <c r="I6" s="7"/>
+      <c r="I6" s="10"/>
       <c r="J6" s="1">
         <v>13</v>
       </c>
-      <c r="K6" s="5">
+      <c r="K6" s="3">
         <v>2583</v>
       </c>
-      <c r="L6" s="11"/>
-      <c r="M6" s="7"/>
+      <c r="L6" s="6"/>
+      <c r="M6" s="10"/>
       <c r="N6" s="1">
         <v>15</v>
       </c>
-      <c r="O6" s="5">
+      <c r="O6" s="3">
         <v>2415</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="3"/>
+      <c r="A7" s="12"/>
       <c r="B7" s="1">
         <v>17</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="3">
         <v>2613</v>
       </c>
-      <c r="D7" s="11"/>
-      <c r="E7" s="7"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="10"/>
       <c r="F7" s="1">
         <v>19</v>
       </c>
-      <c r="G7" s="5">
+      <c r="G7" s="3">
         <v>2425</v>
       </c>
-      <c r="I7" s="7"/>
+      <c r="I7" s="10"/>
       <c r="J7" s="1">
         <v>17</v>
       </c>
-      <c r="K7" s="5">
+      <c r="K7" s="3">
         <v>2604</v>
       </c>
-      <c r="L7" s="11"/>
-      <c r="M7" s="7"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="10"/>
       <c r="N7" s="1">
         <v>19</v>
       </c>
-      <c r="O7" s="5">
+      <c r="O7" s="3">
         <v>2419</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="3"/>
+      <c r="A8" s="12"/>
       <c r="B8" s="1">
         <v>21</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="3">
         <v>2621</v>
       </c>
-      <c r="D8" s="11"/>
-      <c r="E8" s="7"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="10"/>
       <c r="F8" s="1">
         <v>23</v>
       </c>
-      <c r="G8" s="5">
+      <c r="G8" s="3">
         <v>2429</v>
       </c>
-      <c r="I8" s="7"/>
+      <c r="I8" s="10"/>
       <c r="J8" s="1">
         <v>21</v>
       </c>
-      <c r="K8" s="5">
+      <c r="K8" s="3">
         <v>2566</v>
       </c>
-      <c r="L8" s="11"/>
-      <c r="M8" s="7"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="10"/>
       <c r="N8" s="1">
         <v>23</v>
       </c>
-      <c r="O8" s="5">
+      <c r="O8" s="3">
         <v>2446</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="3"/>
+      <c r="A9" s="12"/>
       <c r="B9" s="1">
         <v>25</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="3">
         <v>2608</v>
       </c>
-      <c r="D9" s="11"/>
-      <c r="E9" s="7"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="10"/>
       <c r="F9" s="1">
         <v>27</v>
       </c>
-      <c r="G9" s="5">
+      <c r="G9" s="3">
         <v>2410</v>
       </c>
-      <c r="I9" s="7"/>
+      <c r="I9" s="10"/>
       <c r="J9" s="1">
         <v>25</v>
       </c>
-      <c r="K9" s="5">
+      <c r="K9" s="3">
         <v>2582</v>
       </c>
-      <c r="L9" s="11"/>
-      <c r="M9" s="7"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="10"/>
       <c r="N9" s="1">
         <v>27</v>
       </c>
-      <c r="O9" s="5">
+      <c r="O9" s="3">
         <v>2438</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="3"/>
+      <c r="A10" s="12"/>
       <c r="B10" s="1">
         <v>29</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="3">
         <v>2631</v>
       </c>
-      <c r="D10" s="11"/>
-      <c r="E10" s="7"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="10"/>
       <c r="F10" s="1">
         <v>31</v>
       </c>
-      <c r="G10" s="5">
+      <c r="G10" s="3">
         <v>2462</v>
       </c>
-      <c r="I10" s="7"/>
+      <c r="I10" s="10"/>
       <c r="J10" s="1">
         <v>29</v>
       </c>
-      <c r="K10" s="5">
+      <c r="K10" s="3">
         <v>2558</v>
       </c>
-      <c r="L10" s="11"/>
-      <c r="M10" s="7"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="10"/>
       <c r="N10" s="1">
         <v>31</v>
       </c>
-      <c r="O10" s="5">
+      <c r="O10" s="3">
         <v>2394</v>
       </c>
     </row>
     <row r="11" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="3"/>
+      <c r="A11" s="12"/>
       <c r="B11" s="1">
         <v>33</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C11" s="3">
         <v>2564</v>
       </c>
-      <c r="D11" s="11"/>
-      <c r="E11" s="7"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="10"/>
       <c r="F11" s="1">
         <v>35</v>
       </c>
-      <c r="G11" s="5">
+      <c r="G11" s="3">
         <v>2443</v>
       </c>
-      <c r="I11" s="7"/>
+      <c r="I11" s="10"/>
       <c r="J11" s="1">
         <v>33</v>
       </c>
-      <c r="K11" s="5">
+      <c r="K11" s="3">
         <v>2561</v>
       </c>
-      <c r="L11" s="11"/>
-      <c r="M11" s="7"/>
+      <c r="L11" s="6"/>
+      <c r="M11" s="10"/>
       <c r="N11" s="1">
         <v>35</v>
       </c>
-      <c r="O11" s="5">
+      <c r="O11" s="3">
         <v>2423</v>
       </c>
     </row>
     <row r="12" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="3"/>
+      <c r="A12" s="12"/>
       <c r="B12" s="1">
         <v>37</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12" s="3">
         <v>2571</v>
       </c>
-      <c r="D12" s="11"/>
-      <c r="E12" s="7"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="10"/>
       <c r="F12" s="1">
         <v>39</v>
       </c>
-      <c r="G12" s="5">
+      <c r="G12" s="3">
         <v>2450</v>
       </c>
-      <c r="I12" s="7"/>
+      <c r="I12" s="10"/>
       <c r="J12" s="1">
         <v>37</v>
       </c>
-      <c r="K12" s="5">
+      <c r="K12" s="3">
         <v>2620</v>
       </c>
-      <c r="L12" s="11"/>
-      <c r="M12" s="7"/>
+      <c r="L12" s="6"/>
+      <c r="M12" s="10"/>
       <c r="N12" s="1">
         <v>39</v>
       </c>
-      <c r="O12" s="5">
+      <c r="O12" s="3">
         <v>2424</v>
       </c>
     </row>
     <row r="13" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="3"/>
+      <c r="A13" s="12"/>
       <c r="B13" s="1">
         <v>41</v>
       </c>
-      <c r="C13" s="5">
+      <c r="C13" s="3">
         <v>2586</v>
       </c>
-      <c r="D13" s="11"/>
-      <c r="E13" s="7"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="10"/>
       <c r="F13" s="1">
         <v>43</v>
       </c>
-      <c r="G13" s="5">
+      <c r="G13" s="3">
         <v>2406</v>
       </c>
-      <c r="I13" s="8"/>
+      <c r="I13" s="11"/>
       <c r="J13" s="1">
         <v>41</v>
       </c>
-      <c r="K13" s="5">
+      <c r="K13" s="3">
         <v>2599</v>
       </c>
-      <c r="L13" s="11"/>
-      <c r="M13" s="8"/>
+      <c r="L13" s="6"/>
+      <c r="M13" s="11"/>
       <c r="N13" s="1">
         <v>43</v>
       </c>
-      <c r="O13" s="5">
+      <c r="O13" s="3">
         <v>2421</v>
       </c>
     </row>
     <row r="14" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="3"/>
+      <c r="A14" s="12"/>
       <c r="B14" s="1">
         <v>45</v>
       </c>
-      <c r="C14" s="5">
+      <c r="C14" s="3">
         <v>2601</v>
       </c>
-      <c r="D14" s="11"/>
-      <c r="E14" s="7"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="10"/>
       <c r="F14" s="1">
         <v>47</v>
       </c>
-      <c r="G14" s="5">
+      <c r="G14" s="3">
         <v>2472</v>
       </c>
-      <c r="I14" s="6" t="s">
+      <c r="I14" s="9" t="s">
         <v>5</v>
       </c>
       <c r="J14" s="1">
         <v>2</v>
       </c>
-      <c r="K14" s="5">
+      <c r="K14" s="3">
         <v>2368</v>
       </c>
-      <c r="L14" s="11"/>
-      <c r="M14" s="6" t="s">
+      <c r="L14" s="6"/>
+      <c r="M14" s="9" t="s">
         <v>7</v>
       </c>
       <c r="N14" s="1">
         <v>4</v>
       </c>
-      <c r="O14" s="5">
+      <c r="O14" s="3">
         <v>2753</v>
       </c>
     </row>
     <row r="15" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="3"/>
+      <c r="A15" s="12"/>
       <c r="B15" s="1">
         <v>49</v>
       </c>
-      <c r="C15" s="5">
+      <c r="C15" s="3">
         <v>2563</v>
       </c>
-      <c r="D15" s="11"/>
-      <c r="E15" s="7"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="10"/>
       <c r="F15" s="1">
         <v>51</v>
       </c>
-      <c r="G15" s="5">
+      <c r="G15" s="3">
         <v>2424</v>
       </c>
-      <c r="I15" s="7"/>
+      <c r="I15" s="10"/>
       <c r="J15" s="1">
         <v>6</v>
       </c>
-      <c r="K15" s="5">
+      <c r="K15" s="3">
         <v>2382</v>
       </c>
-      <c r="L15" s="11"/>
-      <c r="M15" s="7"/>
+      <c r="L15" s="6"/>
+      <c r="M15" s="10"/>
       <c r="N15" s="1">
         <v>8</v>
       </c>
-      <c r="O15" s="5">
+      <c r="O15" s="3">
         <v>2688</v>
       </c>
     </row>
     <row r="16" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="3"/>
+      <c r="A16" s="12"/>
       <c r="B16" s="1">
         <v>53</v>
       </c>
-      <c r="C16" s="5">
+      <c r="C16" s="3">
         <v>2613</v>
       </c>
-      <c r="D16" s="11"/>
-      <c r="E16" s="7"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="10"/>
       <c r="F16" s="1">
         <v>55</v>
       </c>
-      <c r="G16" s="5">
+      <c r="G16" s="3">
         <v>2469</v>
       </c>
-      <c r="I16" s="7"/>
+      <c r="I16" s="10"/>
       <c r="J16" s="1">
         <v>10</v>
       </c>
-      <c r="K16" s="5">
+      <c r="K16" s="3">
         <v>2389</v>
       </c>
-      <c r="L16" s="11"/>
-      <c r="M16" s="7"/>
+      <c r="L16" s="6"/>
+      <c r="M16" s="10"/>
       <c r="N16" s="1">
         <v>12</v>
       </c>
-      <c r="O16" s="5">
+      <c r="O16" s="3">
         <v>2773</v>
       </c>
     </row>
     <row r="17" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="3"/>
+      <c r="A17" s="12"/>
       <c r="B17" s="1">
         <v>57</v>
       </c>
-      <c r="C17" s="5">
+      <c r="C17" s="3">
         <v>2624</v>
       </c>
-      <c r="D17" s="11"/>
-      <c r="E17" s="7"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="10"/>
       <c r="F17" s="1">
         <v>59</v>
       </c>
-      <c r="G17" s="5">
+      <c r="G17" s="3">
         <v>2413</v>
       </c>
-      <c r="I17" s="7"/>
+      <c r="I17" s="10"/>
       <c r="J17" s="1">
         <v>14</v>
       </c>
-      <c r="K17" s="5">
+      <c r="K17" s="3">
         <v>2411</v>
       </c>
-      <c r="L17" s="11"/>
-      <c r="M17" s="7"/>
+      <c r="L17" s="6"/>
+      <c r="M17" s="10"/>
       <c r="N17" s="1">
         <v>16</v>
       </c>
-      <c r="O17" s="5">
+      <c r="O17" s="3">
         <v>2741</v>
       </c>
     </row>
     <row r="18" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="3"/>
+      <c r="A18" s="12"/>
       <c r="B18" s="1">
         <v>61</v>
       </c>
-      <c r="C18" s="5">
+      <c r="C18" s="3">
         <v>2549</v>
       </c>
-      <c r="D18" s="11"/>
-      <c r="E18" s="8"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="11"/>
       <c r="F18" s="1">
         <v>63</v>
       </c>
-      <c r="G18" s="5">
+      <c r="G18" s="3">
         <v>2440</v>
       </c>
-      <c r="I18" s="7"/>
+      <c r="I18" s="10"/>
       <c r="J18" s="1">
         <v>18</v>
       </c>
-      <c r="K18" s="5">
+      <c r="K18" s="3">
         <v>2406</v>
       </c>
-      <c r="L18" s="11"/>
-      <c r="M18" s="7"/>
+      <c r="L18" s="6"/>
+      <c r="M18" s="10"/>
       <c r="N18" s="1">
         <v>20</v>
       </c>
-      <c r="O18" s="5">
+      <c r="O18" s="3">
         <v>2692</v>
       </c>
     </row>
     <row r="19" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="3" t="s">
+      <c r="A19" s="12" t="s">
         <v>5</v>
       </c>
       <c r="B19" s="1">
         <v>2</v>
       </c>
-      <c r="C19" s="5">
+      <c r="C19" s="3">
         <v>2438</v>
       </c>
-      <c r="D19" s="11"/>
-      <c r="E19" s="6" t="s">
+      <c r="D19" s="6"/>
+      <c r="E19" s="9" t="s">
         <v>7</v>
       </c>
       <c r="F19" s="1">
         <v>4</v>
       </c>
-      <c r="G19" s="5">
+      <c r="G19" s="3">
         <v>2779</v>
       </c>
-      <c r="I19" s="7"/>
+      <c r="I19" s="10"/>
       <c r="J19" s="1">
         <v>22</v>
       </c>
-      <c r="K19" s="5">
+      <c r="K19" s="3">
         <v>2412</v>
       </c>
-      <c r="L19" s="11"/>
-      <c r="M19" s="7"/>
+      <c r="L19" s="6"/>
+      <c r="M19" s="10"/>
       <c r="N19" s="1">
         <v>24</v>
       </c>
-      <c r="O19" s="5">
+      <c r="O19" s="3">
         <v>2740</v>
       </c>
     </row>
     <row r="20" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="3"/>
+      <c r="A20" s="12"/>
       <c r="B20" s="1">
         <v>6</v>
       </c>
-      <c r="C20" s="5">
+      <c r="C20" s="3">
         <v>2411</v>
       </c>
-      <c r="D20" s="11"/>
-      <c r="E20" s="7"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="10"/>
       <c r="F20" s="1">
         <v>8</v>
       </c>
-      <c r="G20" s="5">
+      <c r="G20" s="3">
         <v>2681</v>
       </c>
-      <c r="I20" s="7"/>
+      <c r="I20" s="10"/>
       <c r="J20" s="1">
         <v>26</v>
       </c>
-      <c r="K20" s="5">
+      <c r="K20" s="3">
         <v>2386</v>
       </c>
-      <c r="L20" s="11"/>
-      <c r="M20" s="7"/>
+      <c r="L20" s="6"/>
+      <c r="M20" s="10"/>
       <c r="N20" s="1">
         <v>28</v>
       </c>
-      <c r="O20" s="5">
+      <c r="O20" s="3">
         <v>2737</v>
       </c>
     </row>
     <row r="21" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="3"/>
+      <c r="A21" s="12"/>
       <c r="B21" s="1">
         <v>10</v>
       </c>
-      <c r="C21" s="5">
+      <c r="C21" s="3">
         <v>2384</v>
       </c>
-      <c r="D21" s="11"/>
-      <c r="E21" s="7"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="10"/>
       <c r="F21" s="1">
         <v>12</v>
       </c>
-      <c r="G21" s="5">
+      <c r="G21" s="3">
         <v>2667</v>
       </c>
-      <c r="I21" s="7"/>
+      <c r="I21" s="10"/>
       <c r="J21" s="1">
         <v>30</v>
       </c>
-      <c r="K21" s="5">
+      <c r="K21" s="3">
         <v>2390</v>
       </c>
-      <c r="L21" s="11"/>
-      <c r="M21" s="7"/>
+      <c r="L21" s="6"/>
+      <c r="M21" s="10"/>
       <c r="N21" s="1">
         <v>32</v>
       </c>
-      <c r="O21" s="5">
+      <c r="O21" s="3">
         <v>2676</v>
       </c>
     </row>
     <row r="22" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="3"/>
+      <c r="A22" s="12"/>
       <c r="B22" s="1">
         <v>14</v>
       </c>
-      <c r="C22" s="5">
+      <c r="C22" s="3">
         <v>2422</v>
       </c>
-      <c r="D22" s="11"/>
-      <c r="E22" s="7"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="10"/>
       <c r="F22" s="1">
         <v>16</v>
       </c>
-      <c r="G22" s="5">
+      <c r="G22" s="3">
         <v>2785</v>
       </c>
-      <c r="I22" s="7"/>
+      <c r="I22" s="10"/>
       <c r="J22" s="1">
         <v>34</v>
       </c>
-      <c r="K22" s="5">
+      <c r="K22" s="3">
         <v>2429</v>
       </c>
-      <c r="L22" s="11"/>
-      <c r="M22" s="7"/>
+      <c r="L22" s="6"/>
+      <c r="M22" s="10"/>
       <c r="N22" s="1">
         <v>36</v>
       </c>
-      <c r="O22" s="5">
+      <c r="O22" s="3">
         <v>2725</v>
       </c>
     </row>
     <row r="23" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="3"/>
+      <c r="A23" s="12"/>
       <c r="B23" s="1">
         <v>18</v>
       </c>
-      <c r="C23" s="5">
+      <c r="C23" s="3">
         <v>2398</v>
       </c>
-      <c r="D23" s="11"/>
-      <c r="E23" s="7"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="10"/>
       <c r="F23" s="1">
         <v>20</v>
       </c>
-      <c r="G23" s="5">
+      <c r="G23" s="3">
         <v>2668</v>
       </c>
-      <c r="I23" s="7"/>
+      <c r="I23" s="10"/>
       <c r="J23" s="1">
         <v>38</v>
       </c>
-      <c r="K23" s="5">
+      <c r="K23" s="3">
         <v>2399</v>
       </c>
-      <c r="L23" s="11"/>
-      <c r="M23" s="7"/>
+      <c r="L23" s="6"/>
+      <c r="M23" s="10"/>
       <c r="N23" s="1">
         <v>40</v>
       </c>
-      <c r="O23" s="5">
+      <c r="O23" s="3">
         <v>2719</v>
       </c>
     </row>
     <row r="24" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="3"/>
+      <c r="A24" s="12"/>
       <c r="B24" s="1">
         <v>22</v>
       </c>
-      <c r="C24" s="5">
+      <c r="C24" s="3">
         <v>2421</v>
       </c>
-      <c r="D24" s="11"/>
-      <c r="E24" s="7"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="10"/>
       <c r="F24" s="1">
         <v>24</v>
       </c>
-      <c r="G24" s="5">
+      <c r="G24" s="3">
         <v>2711</v>
       </c>
-      <c r="I24" s="8"/>
+      <c r="I24" s="11"/>
       <c r="J24" s="1">
         <v>42</v>
       </c>
-      <c r="K24" s="5">
+      <c r="K24" s="3">
         <v>2392</v>
       </c>
-      <c r="L24" s="12"/>
-      <c r="M24" s="8"/>
+      <c r="L24" s="7"/>
+      <c r="M24" s="11"/>
       <c r="N24" s="1">
         <v>44</v>
       </c>
-      <c r="O24" s="5">
+      <c r="O24" s="3">
         <v>2672</v>
       </c>
     </row>
     <row r="25" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="3"/>
+      <c r="A25" s="12"/>
       <c r="B25" s="1">
         <v>26</v>
       </c>
-      <c r="C25" s="5">
+      <c r="C25" s="3">
         <v>2414</v>
       </c>
-      <c r="D25" s="11"/>
-      <c r="E25" s="7"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="10"/>
       <c r="F25" s="1">
         <v>28</v>
       </c>
-      <c r="G25" s="5">
+      <c r="G25" s="3">
         <v>2794</v>
       </c>
     </row>
     <row r="26" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="3"/>
+      <c r="A26" s="12"/>
       <c r="B26" s="1">
         <v>30</v>
       </c>
-      <c r="C26" s="5">
+      <c r="C26" s="3">
         <v>2425</v>
       </c>
-      <c r="D26" s="11"/>
-      <c r="E26" s="7"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="10"/>
       <c r="F26" s="1">
         <v>32</v>
       </c>
-      <c r="G26" s="5">
+      <c r="G26" s="3">
         <v>2712</v>
       </c>
     </row>
     <row r="27" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="3"/>
+      <c r="A27" s="12"/>
       <c r="B27" s="1">
         <v>34</v>
       </c>
-      <c r="C27" s="5">
+      <c r="C27" s="3">
         <v>2420</v>
       </c>
-      <c r="D27" s="11"/>
-      <c r="E27" s="7"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="10"/>
       <c r="F27" s="1">
         <v>36</v>
       </c>
-      <c r="G27" s="5">
+      <c r="G27" s="3">
         <v>2741</v>
       </c>
     </row>
     <row r="28" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="3"/>
+      <c r="A28" s="12"/>
       <c r="B28" s="1">
         <v>38</v>
       </c>
-      <c r="C28" s="5">
+      <c r="C28" s="3">
         <v>2414</v>
       </c>
-      <c r="D28" s="11"/>
-      <c r="E28" s="7"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="10"/>
       <c r="F28" s="1">
         <v>40</v>
       </c>
-      <c r="G28" s="5">
+      <c r="G28" s="3">
         <v>2804</v>
       </c>
     </row>
     <row r="29" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="3"/>
+      <c r="A29" s="12"/>
       <c r="B29" s="1">
         <v>42</v>
       </c>
-      <c r="C29" s="5">
+      <c r="C29" s="3">
         <v>2389</v>
       </c>
-      <c r="D29" s="11"/>
-      <c r="E29" s="7"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="10"/>
       <c r="F29" s="1">
         <v>44</v>
       </c>
-      <c r="G29" s="5">
+      <c r="G29" s="3">
         <v>2727</v>
       </c>
     </row>
     <row r="30" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="3"/>
+      <c r="A30" s="12"/>
       <c r="B30" s="1">
         <v>46</v>
       </c>
-      <c r="C30" s="5">
+      <c r="C30" s="3">
         <v>2397</v>
       </c>
-      <c r="D30" s="11"/>
-      <c r="E30" s="7"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="10"/>
       <c r="F30" s="1">
         <v>48</v>
       </c>
-      <c r="G30" s="5">
+      <c r="G30" s="3">
         <v>2722</v>
       </c>
     </row>
     <row r="31" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="3"/>
+      <c r="A31" s="12"/>
       <c r="B31" s="1">
         <v>50</v>
       </c>
-      <c r="C31" s="5">
+      <c r="C31" s="3">
         <v>2409</v>
       </c>
-      <c r="D31" s="11"/>
-      <c r="E31" s="7"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="10"/>
       <c r="F31" s="1">
         <v>52</v>
       </c>
-      <c r="G31" s="5">
+      <c r="G31" s="3">
         <v>2710</v>
       </c>
     </row>
     <row r="32" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="3"/>
+      <c r="A32" s="12"/>
       <c r="B32" s="1">
         <v>54</v>
       </c>
-      <c r="C32" s="5">
+      <c r="C32" s="3">
         <v>2416</v>
       </c>
-      <c r="D32" s="11"/>
-      <c r="E32" s="7"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="10"/>
       <c r="F32" s="1">
         <v>56</v>
       </c>
-      <c r="G32" s="5">
+      <c r="G32" s="3">
         <v>2739</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="3"/>
+      <c r="A33" s="12"/>
       <c r="B33" s="1">
         <v>58</v>
       </c>
-      <c r="C33" s="5">
+      <c r="C33" s="3">
         <v>2433</v>
       </c>
-      <c r="D33" s="11"/>
-      <c r="E33" s="7"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="10"/>
       <c r="F33" s="1">
         <v>60</v>
       </c>
-      <c r="G33" s="5">
+      <c r="G33" s="3">
         <v>2704</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="3"/>
+      <c r="A34" s="12"/>
       <c r="B34" s="1">
         <v>62</v>
       </c>
-      <c r="C34" s="5">
+      <c r="C34" s="3">
         <v>2409</v>
       </c>
-      <c r="D34" s="12"/>
-      <c r="E34" s="8"/>
+      <c r="D34" s="7"/>
+      <c r="E34" s="11"/>
       <c r="F34" s="1">
         <v>64</v>
       </c>
-      <c r="G34" s="5">
+      <c r="G34" s="3">
         <v>2761</v>
       </c>
     </row>
@@ -3560,4 +3825,1166 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4C523F4-74B3-4E7D-8BAC-552A17169E6B}">
+  <dimension ref="A1:U34"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="S25" sqref="S25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8.6640625" customWidth="1"/>
+    <col min="18" max="18" width="8.44140625" customWidth="1"/>
+    <col min="19" max="21" width="10.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="I1" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12"/>
+      <c r="O1" s="12"/>
+      <c r="Q1" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="R1" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="S1" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="T1" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="U1" s="24" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" ht="18" x14ac:dyDescent="0.35">
+      <c r="A2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="8"/>
+      <c r="E2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="2"/>
+      <c r="I2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="L2" s="5"/>
+      <c r="M2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q2" s="25">
+        <v>1</v>
+      </c>
+      <c r="R2" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="S2" s="27">
+        <f>AVERAGE($C$3:$C$18)</f>
+        <v>2587.0625</v>
+      </c>
+      <c r="T2" s="28">
+        <f>_xlfn.STDEV.S($C$3:$C$18)</f>
+        <v>29.672588360303184</v>
+      </c>
+      <c r="U2" s="29">
+        <f>COUNT($C$3:$C$18)</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" ht="18" x14ac:dyDescent="0.35">
+      <c r="A3" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" s="3">
+        <v>2565</v>
+      </c>
+      <c r="D3" s="6"/>
+      <c r="E3" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="1">
+        <v>3</v>
+      </c>
+      <c r="G3" s="3">
+        <v>2441</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="J3" s="1">
+        <v>1</v>
+      </c>
+      <c r="K3" s="37">
+        <v>2393</v>
+      </c>
+      <c r="L3" s="6"/>
+      <c r="M3" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="N3" s="1">
+        <v>3</v>
+      </c>
+      <c r="O3" s="3">
+        <v>2438</v>
+      </c>
+      <c r="Q3" s="17"/>
+      <c r="R3" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="S3" s="14">
+        <f>AVERAGE($C$19:$C$34)</f>
+        <v>2412.5</v>
+      </c>
+      <c r="T3" s="15">
+        <f>_xlfn.STDEV.S($C$19:$C$34)</f>
+        <v>14.841383583300672</v>
+      </c>
+      <c r="U3" s="16">
+        <f>COUNT($C$19:$C$34)</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" ht="18" x14ac:dyDescent="0.35">
+      <c r="A4" s="12"/>
+      <c r="B4" s="1">
+        <v>5</v>
+      </c>
+      <c r="C4" s="3">
+        <v>2532</v>
+      </c>
+      <c r="D4" s="6"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="1">
+        <v>7</v>
+      </c>
+      <c r="G4" s="3">
+        <v>2436</v>
+      </c>
+      <c r="I4" s="10"/>
+      <c r="J4" s="1">
+        <v>5</v>
+      </c>
+      <c r="K4" s="3">
+        <v>2550</v>
+      </c>
+      <c r="L4" s="6"/>
+      <c r="M4" s="10"/>
+      <c r="N4" s="1">
+        <v>7</v>
+      </c>
+      <c r="O4" s="3">
+        <v>2439</v>
+      </c>
+      <c r="Q4" s="17"/>
+      <c r="R4" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="S4" s="14">
+        <f>AVERAGE($G$3:$G$18)</f>
+        <v>2437.4375</v>
+      </c>
+      <c r="T4" s="15">
+        <f>_xlfn.STDEV.S($G$3:$G$18)</f>
+        <v>19.599213419590765</v>
+      </c>
+      <c r="U4" s="16">
+        <f>COUNT($G$3:$G$18)</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="12"/>
+      <c r="B5" s="1">
+        <v>9</v>
+      </c>
+      <c r="C5" s="3">
+        <v>2566</v>
+      </c>
+      <c r="D5" s="6"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="1">
+        <v>11</v>
+      </c>
+      <c r="G5" s="3">
+        <v>2441</v>
+      </c>
+      <c r="I5" s="10"/>
+      <c r="J5" s="1">
+        <v>9</v>
+      </c>
+      <c r="K5" s="3">
+        <v>2599</v>
+      </c>
+      <c r="L5" s="6"/>
+      <c r="M5" s="10"/>
+      <c r="N5" s="1">
+        <v>11</v>
+      </c>
+      <c r="O5" s="3">
+        <v>2460</v>
+      </c>
+      <c r="Q5" s="30"/>
+      <c r="R5" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="S5" s="18">
+        <f>AVERAGE($G$19:$G$34)</f>
+        <v>2731.5625</v>
+      </c>
+      <c r="T5" s="19">
+        <f>_xlfn.STDEV.S($G$19:$G$34)</f>
+        <v>43.335849285935694</v>
+      </c>
+      <c r="U5" s="20">
+        <f>COUNT($G$19:$G$34)</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" ht="18" x14ac:dyDescent="0.35">
+      <c r="A6" s="12"/>
+      <c r="B6" s="1">
+        <v>13</v>
+      </c>
+      <c r="C6" s="3">
+        <v>2586</v>
+      </c>
+      <c r="D6" s="6"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="1">
+        <v>15</v>
+      </c>
+      <c r="G6" s="3">
+        <v>2438</v>
+      </c>
+      <c r="I6" s="10"/>
+      <c r="J6" s="1">
+        <v>13</v>
+      </c>
+      <c r="K6" s="3">
+        <v>2583</v>
+      </c>
+      <c r="L6" s="6"/>
+      <c r="M6" s="10"/>
+      <c r="N6" s="1">
+        <v>15</v>
+      </c>
+      <c r="O6" s="3">
+        <v>2415</v>
+      </c>
+      <c r="Q6" s="25">
+        <v>2</v>
+      </c>
+      <c r="R6" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="S6" s="27">
+        <f>AVERAGE($K$4:$K$13)</f>
+        <v>2582.1999999999998</v>
+      </c>
+      <c r="T6" s="28">
+        <f>_xlfn.STDEV.S($K$4:$K$13)</f>
+        <v>23.102669398433882</v>
+      </c>
+      <c r="U6" s="29">
+        <f>COUNT($K$4:$K$13)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" ht="18" x14ac:dyDescent="0.35">
+      <c r="A7" s="12"/>
+      <c r="B7" s="1">
+        <v>17</v>
+      </c>
+      <c r="C7" s="3">
+        <v>2613</v>
+      </c>
+      <c r="D7" s="6"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="1">
+        <v>19</v>
+      </c>
+      <c r="G7" s="3">
+        <v>2425</v>
+      </c>
+      <c r="I7" s="10"/>
+      <c r="J7" s="1">
+        <v>17</v>
+      </c>
+      <c r="K7" s="3">
+        <v>2604</v>
+      </c>
+      <c r="L7" s="6"/>
+      <c r="M7" s="10"/>
+      <c r="N7" s="1">
+        <v>19</v>
+      </c>
+      <c r="O7" s="3">
+        <v>2419</v>
+      </c>
+      <c r="Q7" s="17"/>
+      <c r="R7" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="S7" s="14">
+        <f>AVERAGE($K$14:$K$24)</f>
+        <v>2396.7272727272725</v>
+      </c>
+      <c r="T7" s="15">
+        <f>_xlfn.STDEV.S($K$14:$K$24)</f>
+        <v>16.894323952682505</v>
+      </c>
+      <c r="U7" s="16">
+        <f>COUNT($K$14:$K$24)</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" ht="18" x14ac:dyDescent="0.35">
+      <c r="A8" s="12"/>
+      <c r="B8" s="1">
+        <v>21</v>
+      </c>
+      <c r="C8" s="3">
+        <v>2621</v>
+      </c>
+      <c r="D8" s="6"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="1">
+        <v>23</v>
+      </c>
+      <c r="G8" s="3">
+        <v>2429</v>
+      </c>
+      <c r="I8" s="10"/>
+      <c r="J8" s="1">
+        <v>21</v>
+      </c>
+      <c r="K8" s="3">
+        <v>2566</v>
+      </c>
+      <c r="L8" s="6"/>
+      <c r="M8" s="10"/>
+      <c r="N8" s="1">
+        <v>23</v>
+      </c>
+      <c r="O8" s="3">
+        <v>2446</v>
+      </c>
+      <c r="Q8" s="17"/>
+      <c r="R8" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="S8" s="14">
+        <f>AVERAGE($O$3:$O$13)</f>
+        <v>2428.818181818182</v>
+      </c>
+      <c r="T8" s="15">
+        <f>_xlfn.STDEV.S($O$3:$O$13)</f>
+        <v>17.769739344279539</v>
+      </c>
+      <c r="U8" s="16">
+        <f>COUNT($O$3:$O$13)</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="12"/>
+      <c r="B9" s="1">
+        <v>25</v>
+      </c>
+      <c r="C9" s="3">
+        <v>2608</v>
+      </c>
+      <c r="D9" s="6"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="1">
+        <v>27</v>
+      </c>
+      <c r="G9" s="3">
+        <v>2410</v>
+      </c>
+      <c r="I9" s="10"/>
+      <c r="J9" s="1">
+        <v>25</v>
+      </c>
+      <c r="K9" s="3">
+        <v>2582</v>
+      </c>
+      <c r="L9" s="6"/>
+      <c r="M9" s="10"/>
+      <c r="N9" s="1">
+        <v>27</v>
+      </c>
+      <c r="O9" s="3">
+        <v>2438</v>
+      </c>
+      <c r="Q9" s="30"/>
+      <c r="R9" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="S9" s="18">
+        <f>AVERAGE($O$14:$O$24)</f>
+        <v>2719.6363636363635</v>
+      </c>
+      <c r="T9" s="19">
+        <f>_xlfn.STDEV.S($O$14:$O$24)</f>
+        <v>33.317481079075371</v>
+      </c>
+      <c r="U9" s="20">
+        <f>COUNT($O$14:$O$24)</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="12"/>
+      <c r="B10" s="1">
+        <v>29</v>
+      </c>
+      <c r="C10" s="3">
+        <v>2631</v>
+      </c>
+      <c r="D10" s="6"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="1">
+        <v>31</v>
+      </c>
+      <c r="G10" s="3">
+        <v>2462</v>
+      </c>
+      <c r="I10" s="10"/>
+      <c r="J10" s="1">
+        <v>29</v>
+      </c>
+      <c r="K10" s="3">
+        <v>2558</v>
+      </c>
+      <c r="L10" s="6"/>
+      <c r="M10" s="10"/>
+      <c r="N10" s="1">
+        <v>31</v>
+      </c>
+      <c r="O10" s="3">
+        <v>2394</v>
+      </c>
+      <c r="Q10" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="R10" s="33"/>
+      <c r="S10" s="34">
+        <f>AVERAGE(S2:S9)</f>
+        <v>2536.9930397727271</v>
+      </c>
+      <c r="T10" s="35">
+        <f>_xlfn.STDEV.S($C$3:$C$34,$G$3:$G$34,$K$3:$K$24,$O$3:$O$24)</f>
+        <v>132.47919662702068</v>
+      </c>
+      <c r="U10" s="36">
+        <f>SUM(U2:U9)</f>
+        <v>107</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A11" s="12"/>
+      <c r="B11" s="1">
+        <v>33</v>
+      </c>
+      <c r="C11" s="3">
+        <v>2564</v>
+      </c>
+      <c r="D11" s="6"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="1">
+        <v>35</v>
+      </c>
+      <c r="G11" s="3">
+        <v>2443</v>
+      </c>
+      <c r="I11" s="10"/>
+      <c r="J11" s="1">
+        <v>33</v>
+      </c>
+      <c r="K11" s="3">
+        <v>2561</v>
+      </c>
+      <c r="L11" s="6"/>
+      <c r="M11" s="10"/>
+      <c r="N11" s="1">
+        <v>35</v>
+      </c>
+      <c r="O11" s="3">
+        <v>2423</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A12" s="12"/>
+      <c r="B12" s="1">
+        <v>37</v>
+      </c>
+      <c r="C12" s="3">
+        <v>2571</v>
+      </c>
+      <c r="D12" s="6"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="1">
+        <v>39</v>
+      </c>
+      <c r="G12" s="3">
+        <v>2450</v>
+      </c>
+      <c r="I12" s="10"/>
+      <c r="J12" s="1">
+        <v>37</v>
+      </c>
+      <c r="K12" s="3">
+        <v>2620</v>
+      </c>
+      <c r="L12" s="6"/>
+      <c r="M12" s="10"/>
+      <c r="N12" s="1">
+        <v>39</v>
+      </c>
+      <c r="O12" s="3">
+        <v>2424</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A13" s="12"/>
+      <c r="B13" s="1">
+        <v>41</v>
+      </c>
+      <c r="C13" s="3">
+        <v>2586</v>
+      </c>
+      <c r="D13" s="6"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="1">
+        <v>43</v>
+      </c>
+      <c r="G13" s="3">
+        <v>2406</v>
+      </c>
+      <c r="I13" s="11"/>
+      <c r="J13" s="1">
+        <v>41</v>
+      </c>
+      <c r="K13" s="3">
+        <v>2599</v>
+      </c>
+      <c r="L13" s="6"/>
+      <c r="M13" s="11"/>
+      <c r="N13" s="1">
+        <v>43</v>
+      </c>
+      <c r="O13" s="3">
+        <v>2421</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A14" s="12"/>
+      <c r="B14" s="1">
+        <v>45</v>
+      </c>
+      <c r="C14" s="3">
+        <v>2601</v>
+      </c>
+      <c r="D14" s="6"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="1">
+        <v>47</v>
+      </c>
+      <c r="G14" s="3">
+        <v>2472</v>
+      </c>
+      <c r="I14" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="J14" s="1">
+        <v>2</v>
+      </c>
+      <c r="K14" s="3">
+        <v>2368</v>
+      </c>
+      <c r="L14" s="6"/>
+      <c r="M14" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="N14" s="1">
+        <v>4</v>
+      </c>
+      <c r="O14" s="3">
+        <v>2753</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A15" s="12"/>
+      <c r="B15" s="1">
+        <v>49</v>
+      </c>
+      <c r="C15" s="3">
+        <v>2563</v>
+      </c>
+      <c r="D15" s="6"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="1">
+        <v>51</v>
+      </c>
+      <c r="G15" s="3">
+        <v>2424</v>
+      </c>
+      <c r="I15" s="10"/>
+      <c r="J15" s="1">
+        <v>6</v>
+      </c>
+      <c r="K15" s="3">
+        <v>2382</v>
+      </c>
+      <c r="L15" s="6"/>
+      <c r="M15" s="10"/>
+      <c r="N15" s="1">
+        <v>8</v>
+      </c>
+      <c r="O15" s="3">
+        <v>2688</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A16" s="12"/>
+      <c r="B16" s="1">
+        <v>53</v>
+      </c>
+      <c r="C16" s="3">
+        <v>2613</v>
+      </c>
+      <c r="D16" s="6"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="1">
+        <v>55</v>
+      </c>
+      <c r="G16" s="3">
+        <v>2469</v>
+      </c>
+      <c r="I16" s="10"/>
+      <c r="J16" s="1">
+        <v>10</v>
+      </c>
+      <c r="K16" s="3">
+        <v>2389</v>
+      </c>
+      <c r="L16" s="6"/>
+      <c r="M16" s="10"/>
+      <c r="N16" s="1">
+        <v>12</v>
+      </c>
+      <c r="O16" s="3">
+        <v>2773</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A17" s="12"/>
+      <c r="B17" s="1">
+        <v>57</v>
+      </c>
+      <c r="C17" s="3">
+        <v>2624</v>
+      </c>
+      <c r="D17" s="6"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="1">
+        <v>59</v>
+      </c>
+      <c r="G17" s="3">
+        <v>2413</v>
+      </c>
+      <c r="I17" s="10"/>
+      <c r="J17" s="1">
+        <v>14</v>
+      </c>
+      <c r="K17" s="3">
+        <v>2411</v>
+      </c>
+      <c r="L17" s="6"/>
+      <c r="M17" s="10"/>
+      <c r="N17" s="1">
+        <v>16</v>
+      </c>
+      <c r="O17" s="3">
+        <v>2741</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A18" s="12"/>
+      <c r="B18" s="1">
+        <v>61</v>
+      </c>
+      <c r="C18" s="3">
+        <v>2549</v>
+      </c>
+      <c r="D18" s="6"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="1">
+        <v>63</v>
+      </c>
+      <c r="G18" s="3">
+        <v>2440</v>
+      </c>
+      <c r="I18" s="10"/>
+      <c r="J18" s="1">
+        <v>18</v>
+      </c>
+      <c r="K18" s="3">
+        <v>2406</v>
+      </c>
+      <c r="L18" s="6"/>
+      <c r="M18" s="10"/>
+      <c r="N18" s="1">
+        <v>20</v>
+      </c>
+      <c r="O18" s="3">
+        <v>2692</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A19" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" s="1">
+        <v>2</v>
+      </c>
+      <c r="C19" s="3">
+        <v>2438</v>
+      </c>
+      <c r="D19" s="6"/>
+      <c r="E19" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F19" s="1">
+        <v>4</v>
+      </c>
+      <c r="G19" s="3">
+        <v>2779</v>
+      </c>
+      <c r="I19" s="10"/>
+      <c r="J19" s="1">
+        <v>22</v>
+      </c>
+      <c r="K19" s="3">
+        <v>2412</v>
+      </c>
+      <c r="L19" s="6"/>
+      <c r="M19" s="10"/>
+      <c r="N19" s="1">
+        <v>24</v>
+      </c>
+      <c r="O19" s="3">
+        <v>2740</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A20" s="12"/>
+      <c r="B20" s="1">
+        <v>6</v>
+      </c>
+      <c r="C20" s="3">
+        <v>2411</v>
+      </c>
+      <c r="D20" s="6"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="1">
+        <v>8</v>
+      </c>
+      <c r="G20" s="3">
+        <v>2681</v>
+      </c>
+      <c r="I20" s="10"/>
+      <c r="J20" s="1">
+        <v>26</v>
+      </c>
+      <c r="K20" s="3">
+        <v>2386</v>
+      </c>
+      <c r="L20" s="6"/>
+      <c r="M20" s="10"/>
+      <c r="N20" s="1">
+        <v>28</v>
+      </c>
+      <c r="O20" s="3">
+        <v>2737</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A21" s="12"/>
+      <c r="B21" s="1">
+        <v>10</v>
+      </c>
+      <c r="C21" s="3">
+        <v>2384</v>
+      </c>
+      <c r="D21" s="6"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="1">
+        <v>12</v>
+      </c>
+      <c r="G21" s="3">
+        <v>2667</v>
+      </c>
+      <c r="I21" s="10"/>
+      <c r="J21" s="1">
+        <v>30</v>
+      </c>
+      <c r="K21" s="3">
+        <v>2390</v>
+      </c>
+      <c r="L21" s="6"/>
+      <c r="M21" s="10"/>
+      <c r="N21" s="1">
+        <v>32</v>
+      </c>
+      <c r="O21" s="3">
+        <v>2676</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A22" s="12"/>
+      <c r="B22" s="1">
+        <v>14</v>
+      </c>
+      <c r="C22" s="3">
+        <v>2422</v>
+      </c>
+      <c r="D22" s="6"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="1">
+        <v>16</v>
+      </c>
+      <c r="G22" s="3">
+        <v>2785</v>
+      </c>
+      <c r="I22" s="10"/>
+      <c r="J22" s="1">
+        <v>34</v>
+      </c>
+      <c r="K22" s="3">
+        <v>2429</v>
+      </c>
+      <c r="L22" s="6"/>
+      <c r="M22" s="10"/>
+      <c r="N22" s="1">
+        <v>36</v>
+      </c>
+      <c r="O22" s="3">
+        <v>2725</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A23" s="12"/>
+      <c r="B23" s="1">
+        <v>18</v>
+      </c>
+      <c r="C23" s="3">
+        <v>2398</v>
+      </c>
+      <c r="D23" s="6"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="1">
+        <v>20</v>
+      </c>
+      <c r="G23" s="3">
+        <v>2668</v>
+      </c>
+      <c r="I23" s="10"/>
+      <c r="J23" s="1">
+        <v>38</v>
+      </c>
+      <c r="K23" s="3">
+        <v>2399</v>
+      </c>
+      <c r="L23" s="6"/>
+      <c r="M23" s="10"/>
+      <c r="N23" s="1">
+        <v>40</v>
+      </c>
+      <c r="O23" s="3">
+        <v>2719</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A24" s="12"/>
+      <c r="B24" s="1">
+        <v>22</v>
+      </c>
+      <c r="C24" s="3">
+        <v>2421</v>
+      </c>
+      <c r="D24" s="6"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="1">
+        <v>24</v>
+      </c>
+      <c r="G24" s="3">
+        <v>2711</v>
+      </c>
+      <c r="I24" s="11"/>
+      <c r="J24" s="1">
+        <v>42</v>
+      </c>
+      <c r="K24" s="3">
+        <v>2392</v>
+      </c>
+      <c r="L24" s="7"/>
+      <c r="M24" s="11"/>
+      <c r="N24" s="1">
+        <v>44</v>
+      </c>
+      <c r="O24" s="3">
+        <v>2672</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A25" s="12"/>
+      <c r="B25" s="1">
+        <v>26</v>
+      </c>
+      <c r="C25" s="3">
+        <v>2414</v>
+      </c>
+      <c r="D25" s="6"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="1">
+        <v>28</v>
+      </c>
+      <c r="G25" s="3">
+        <v>2794</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A26" s="12"/>
+      <c r="B26" s="1">
+        <v>30</v>
+      </c>
+      <c r="C26" s="3">
+        <v>2425</v>
+      </c>
+      <c r="D26" s="6"/>
+      <c r="E26" s="10"/>
+      <c r="F26" s="1">
+        <v>32</v>
+      </c>
+      <c r="G26" s="3">
+        <v>2712</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A27" s="12"/>
+      <c r="B27" s="1">
+        <v>34</v>
+      </c>
+      <c r="C27" s="3">
+        <v>2420</v>
+      </c>
+      <c r="D27" s="6"/>
+      <c r="E27" s="10"/>
+      <c r="F27" s="1">
+        <v>36</v>
+      </c>
+      <c r="G27" s="3">
+        <v>2741</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A28" s="12"/>
+      <c r="B28" s="1">
+        <v>38</v>
+      </c>
+      <c r="C28" s="3">
+        <v>2414</v>
+      </c>
+      <c r="D28" s="6"/>
+      <c r="E28" s="10"/>
+      <c r="F28" s="1">
+        <v>40</v>
+      </c>
+      <c r="G28" s="3">
+        <v>2804</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A29" s="12"/>
+      <c r="B29" s="1">
+        <v>42</v>
+      </c>
+      <c r="C29" s="3">
+        <v>2389</v>
+      </c>
+      <c r="D29" s="6"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="1">
+        <v>44</v>
+      </c>
+      <c r="G29" s="3">
+        <v>2727</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A30" s="12"/>
+      <c r="B30" s="1">
+        <v>46</v>
+      </c>
+      <c r="C30" s="3">
+        <v>2397</v>
+      </c>
+      <c r="D30" s="6"/>
+      <c r="E30" s="10"/>
+      <c r="F30" s="1">
+        <v>48</v>
+      </c>
+      <c r="G30" s="3">
+        <v>2722</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A31" s="12"/>
+      <c r="B31" s="1">
+        <v>50</v>
+      </c>
+      <c r="C31" s="3">
+        <v>2409</v>
+      </c>
+      <c r="D31" s="6"/>
+      <c r="E31" s="10"/>
+      <c r="F31" s="1">
+        <v>52</v>
+      </c>
+      <c r="G31" s="3">
+        <v>2710</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A32" s="12"/>
+      <c r="B32" s="1">
+        <v>54</v>
+      </c>
+      <c r="C32" s="3">
+        <v>2416</v>
+      </c>
+      <c r="D32" s="6"/>
+      <c r="E32" s="10"/>
+      <c r="F32" s="1">
+        <v>56</v>
+      </c>
+      <c r="G32" s="3">
+        <v>2739</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A33" s="12"/>
+      <c r="B33" s="1">
+        <v>58</v>
+      </c>
+      <c r="C33" s="3">
+        <v>2433</v>
+      </c>
+      <c r="D33" s="6"/>
+      <c r="E33" s="10"/>
+      <c r="F33" s="1">
+        <v>60</v>
+      </c>
+      <c r="G33" s="3">
+        <v>2704</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A34" s="12"/>
+      <c r="B34" s="1">
+        <v>62</v>
+      </c>
+      <c r="C34" s="3">
+        <v>2409</v>
+      </c>
+      <c r="D34" s="7"/>
+      <c r="E34" s="11"/>
+      <c r="F34" s="1">
+        <v>64</v>
+      </c>
+      <c r="G34" s="3">
+        <v>2761</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="13">
+    <mergeCell ref="Q2:Q5"/>
+    <mergeCell ref="Q6:Q9"/>
+    <mergeCell ref="Q10:R10"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="I1:O1"/>
+    <mergeCell ref="A3:A18"/>
+    <mergeCell ref="E3:E18"/>
+    <mergeCell ref="I3:I13"/>
+    <mergeCell ref="M3:M13"/>
+    <mergeCell ref="I14:I24"/>
+    <mergeCell ref="M14:M24"/>
+    <mergeCell ref="A19:A34"/>
+    <mergeCell ref="E19:E34"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
done for the morning
</commit_message>
<xml_diff>
--- a/velocity.xlsx
+++ b/velocity.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Documents\TAMU\Spring_2023\final_proj\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA72CE8E-7D01-4EA0-92AF-44370854B266}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{878D4B2B-340E-46A7-A8ED-6CB37FE7BF8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12" yWindow="1764" windowWidth="22596" windowHeight="8964" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="velocity" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="22">
   <si>
     <t>cnt</t>
   </si>
@@ -79,9 +79,6 @@
     <t>Rifle</t>
   </si>
   <si>
-    <t>Amo</t>
-  </si>
-  <si>
     <t>n</t>
   </si>
   <si>
@@ -93,13 +90,26 @@
   <si>
     <t>Total</t>
   </si>
+  <si>
+    <t>W Statistic</t>
+  </si>
+  <si>
+    <t>P-value</t>
+  </si>
+  <si>
+    <t>Shapiro-Wilk Test Normality</t>
+  </si>
+  <si>
+    <t>Brown-Forsythe Test (alpha = 0.05)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
+    <numFmt numFmtId="166" formatCode="0.0000"/>
   </numFmts>
   <fonts count="22" x14ac:knownFonts="1">
     <font>
@@ -467,7 +477,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="26">
+  <borders count="32">
     <border>
       <left/>
       <right/>
@@ -798,6 +808,90 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -843,7 +937,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="35" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -859,15 +953,6 @@
     <xf numFmtId="0" fontId="0" fillId="33" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="35" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="35" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="35" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="35" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -877,9 +962,6 @@
     <xf numFmtId="3" fontId="18" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="18" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="18" fillId="34" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="35" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="3" fontId="18" fillId="34" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="18" fillId="34" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="18" fillId="34" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -895,25 +977,13 @@
     <xf numFmtId="0" fontId="18" fillId="35" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="35" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="35" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="18" fillId="34" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="18" fillId="34" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="18" fillId="34" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="35" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="35" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="35" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="35" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="18" fillId="34" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -922,6 +992,102 @@
     <xf numFmtId="3" fontId="21" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="18" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="16" fillId="34" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="35" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="16" fillId="34" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="16" fillId="34" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="35" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -978,6 +1144,99 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>410672</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>19612</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{01F8EE0E-DC66-4853-77B5-6F1C642812A2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17468850" y="133350"/>
+          <a:ext cx="7859222" cy="4029637"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>847725</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>20062</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>134057</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{423FC24E-B937-38AD-A01E-80CFC6573EC2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10058400" y="123825"/>
+          <a:ext cx="7249537" cy="5068007"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2844,24 +3103,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="18" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="I1" s="12" t="s">
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="I1" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
-      <c r="M1" s="12"/>
-      <c r="N1" s="12"/>
-      <c r="O1" s="12"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="33"/>
+      <c r="M1" s="33"/>
+      <c r="N1" s="33"/>
+      <c r="O1" s="33"/>
     </row>
     <row r="2" spans="1:15" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
@@ -2905,7 +3164,7 @@
       </c>
     </row>
     <row r="3" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="33" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="1">
@@ -2915,7 +3174,7 @@
         <v>2565</v>
       </c>
       <c r="D3" s="6"/>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="30" t="s">
         <v>6</v>
       </c>
       <c r="F3" s="1">
@@ -2924,17 +3183,17 @@
       <c r="G3" s="3">
         <v>2441</v>
       </c>
-      <c r="I3" s="9" t="s">
+      <c r="I3" s="30" t="s">
         <v>4</v>
       </c>
       <c r="J3" s="1">
         <v>1</v>
       </c>
-      <c r="K3" s="37">
+      <c r="K3" s="29">
         <v>2393</v>
       </c>
       <c r="L3" s="6"/>
-      <c r="M3" s="9" t="s">
+      <c r="M3" s="30" t="s">
         <v>6</v>
       </c>
       <c r="N3" s="1">
@@ -2945,7 +3204,7 @@
       </c>
     </row>
     <row r="4" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="12"/>
+      <c r="A4" s="33"/>
       <c r="B4" s="1">
         <v>5</v>
       </c>
@@ -2953,14 +3212,14 @@
         <v>2532</v>
       </c>
       <c r="D4" s="6"/>
-      <c r="E4" s="10"/>
+      <c r="E4" s="31"/>
       <c r="F4" s="1">
         <v>7</v>
       </c>
       <c r="G4" s="3">
         <v>2436</v>
       </c>
-      <c r="I4" s="10"/>
+      <c r="I4" s="31"/>
       <c r="J4" s="1">
         <v>5</v>
       </c>
@@ -2968,7 +3227,7 @@
         <v>2550</v>
       </c>
       <c r="L4" s="6"/>
-      <c r="M4" s="10"/>
+      <c r="M4" s="31"/>
       <c r="N4" s="1">
         <v>7</v>
       </c>
@@ -2977,7 +3236,7 @@
       </c>
     </row>
     <row r="5" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="12"/>
+      <c r="A5" s="33"/>
       <c r="B5" s="1">
         <v>9</v>
       </c>
@@ -2985,14 +3244,14 @@
         <v>2566</v>
       </c>
       <c r="D5" s="6"/>
-      <c r="E5" s="10"/>
+      <c r="E5" s="31"/>
       <c r="F5" s="1">
         <v>11</v>
       </c>
       <c r="G5" s="3">
         <v>2441</v>
       </c>
-      <c r="I5" s="10"/>
+      <c r="I5" s="31"/>
       <c r="J5" s="1">
         <v>9</v>
       </c>
@@ -3000,7 +3259,7 @@
         <v>2599</v>
       </c>
       <c r="L5" s="6"/>
-      <c r="M5" s="10"/>
+      <c r="M5" s="31"/>
       <c r="N5" s="1">
         <v>11</v>
       </c>
@@ -3009,7 +3268,7 @@
       </c>
     </row>
     <row r="6" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="12"/>
+      <c r="A6" s="33"/>
       <c r="B6" s="1">
         <v>13</v>
       </c>
@@ -3017,14 +3276,14 @@
         <v>2586</v>
       </c>
       <c r="D6" s="6"/>
-      <c r="E6" s="10"/>
+      <c r="E6" s="31"/>
       <c r="F6" s="1">
         <v>15</v>
       </c>
       <c r="G6" s="3">
         <v>2438</v>
       </c>
-      <c r="I6" s="10"/>
+      <c r="I6" s="31"/>
       <c r="J6" s="1">
         <v>13</v>
       </c>
@@ -3032,7 +3291,7 @@
         <v>2583</v>
       </c>
       <c r="L6" s="6"/>
-      <c r="M6" s="10"/>
+      <c r="M6" s="31"/>
       <c r="N6" s="1">
         <v>15</v>
       </c>
@@ -3041,7 +3300,7 @@
       </c>
     </row>
     <row r="7" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="12"/>
+      <c r="A7" s="33"/>
       <c r="B7" s="1">
         <v>17</v>
       </c>
@@ -3049,14 +3308,14 @@
         <v>2613</v>
       </c>
       <c r="D7" s="6"/>
-      <c r="E7" s="10"/>
+      <c r="E7" s="31"/>
       <c r="F7" s="1">
         <v>19</v>
       </c>
       <c r="G7" s="3">
         <v>2425</v>
       </c>
-      <c r="I7" s="10"/>
+      <c r="I7" s="31"/>
       <c r="J7" s="1">
         <v>17</v>
       </c>
@@ -3064,7 +3323,7 @@
         <v>2604</v>
       </c>
       <c r="L7" s="6"/>
-      <c r="M7" s="10"/>
+      <c r="M7" s="31"/>
       <c r="N7" s="1">
         <v>19</v>
       </c>
@@ -3073,7 +3332,7 @@
       </c>
     </row>
     <row r="8" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="12"/>
+      <c r="A8" s="33"/>
       <c r="B8" s="1">
         <v>21</v>
       </c>
@@ -3081,14 +3340,14 @@
         <v>2621</v>
       </c>
       <c r="D8" s="6"/>
-      <c r="E8" s="10"/>
+      <c r="E8" s="31"/>
       <c r="F8" s="1">
         <v>23</v>
       </c>
       <c r="G8" s="3">
         <v>2429</v>
       </c>
-      <c r="I8" s="10"/>
+      <c r="I8" s="31"/>
       <c r="J8" s="1">
         <v>21</v>
       </c>
@@ -3096,7 +3355,7 @@
         <v>2566</v>
       </c>
       <c r="L8" s="6"/>
-      <c r="M8" s="10"/>
+      <c r="M8" s="31"/>
       <c r="N8" s="1">
         <v>23</v>
       </c>
@@ -3105,7 +3364,7 @@
       </c>
     </row>
     <row r="9" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="12"/>
+      <c r="A9" s="33"/>
       <c r="B9" s="1">
         <v>25</v>
       </c>
@@ -3113,14 +3372,14 @@
         <v>2608</v>
       </c>
       <c r="D9" s="6"/>
-      <c r="E9" s="10"/>
+      <c r="E9" s="31"/>
       <c r="F9" s="1">
         <v>27</v>
       </c>
       <c r="G9" s="3">
         <v>2410</v>
       </c>
-      <c r="I9" s="10"/>
+      <c r="I9" s="31"/>
       <c r="J9" s="1">
         <v>25</v>
       </c>
@@ -3128,7 +3387,7 @@
         <v>2582</v>
       </c>
       <c r="L9" s="6"/>
-      <c r="M9" s="10"/>
+      <c r="M9" s="31"/>
       <c r="N9" s="1">
         <v>27</v>
       </c>
@@ -3137,7 +3396,7 @@
       </c>
     </row>
     <row r="10" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="12"/>
+      <c r="A10" s="33"/>
       <c r="B10" s="1">
         <v>29</v>
       </c>
@@ -3145,14 +3404,14 @@
         <v>2631</v>
       </c>
       <c r="D10" s="6"/>
-      <c r="E10" s="10"/>
+      <c r="E10" s="31"/>
       <c r="F10" s="1">
         <v>31</v>
       </c>
       <c r="G10" s="3">
         <v>2462</v>
       </c>
-      <c r="I10" s="10"/>
+      <c r="I10" s="31"/>
       <c r="J10" s="1">
         <v>29</v>
       </c>
@@ -3160,7 +3419,7 @@
         <v>2558</v>
       </c>
       <c r="L10" s="6"/>
-      <c r="M10" s="10"/>
+      <c r="M10" s="31"/>
       <c r="N10" s="1">
         <v>31</v>
       </c>
@@ -3169,7 +3428,7 @@
       </c>
     </row>
     <row r="11" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="12"/>
+      <c r="A11" s="33"/>
       <c r="B11" s="1">
         <v>33</v>
       </c>
@@ -3177,14 +3436,14 @@
         <v>2564</v>
       </c>
       <c r="D11" s="6"/>
-      <c r="E11" s="10"/>
+      <c r="E11" s="31"/>
       <c r="F11" s="1">
         <v>35</v>
       </c>
       <c r="G11" s="3">
         <v>2443</v>
       </c>
-      <c r="I11" s="10"/>
+      <c r="I11" s="31"/>
       <c r="J11" s="1">
         <v>33</v>
       </c>
@@ -3192,7 +3451,7 @@
         <v>2561</v>
       </c>
       <c r="L11" s="6"/>
-      <c r="M11" s="10"/>
+      <c r="M11" s="31"/>
       <c r="N11" s="1">
         <v>35</v>
       </c>
@@ -3201,7 +3460,7 @@
       </c>
     </row>
     <row r="12" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="12"/>
+      <c r="A12" s="33"/>
       <c r="B12" s="1">
         <v>37</v>
       </c>
@@ -3209,14 +3468,14 @@
         <v>2571</v>
       </c>
       <c r="D12" s="6"/>
-      <c r="E12" s="10"/>
+      <c r="E12" s="31"/>
       <c r="F12" s="1">
         <v>39</v>
       </c>
       <c r="G12" s="3">
         <v>2450</v>
       </c>
-      <c r="I12" s="10"/>
+      <c r="I12" s="31"/>
       <c r="J12" s="1">
         <v>37</v>
       </c>
@@ -3224,7 +3483,7 @@
         <v>2620</v>
       </c>
       <c r="L12" s="6"/>
-      <c r="M12" s="10"/>
+      <c r="M12" s="31"/>
       <c r="N12" s="1">
         <v>39</v>
       </c>
@@ -3233,7 +3492,7 @@
       </c>
     </row>
     <row r="13" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="12"/>
+      <c r="A13" s="33"/>
       <c r="B13" s="1">
         <v>41</v>
       </c>
@@ -3241,14 +3500,14 @@
         <v>2586</v>
       </c>
       <c r="D13" s="6"/>
-      <c r="E13" s="10"/>
+      <c r="E13" s="31"/>
       <c r="F13" s="1">
         <v>43</v>
       </c>
       <c r="G13" s="3">
         <v>2406</v>
       </c>
-      <c r="I13" s="11"/>
+      <c r="I13" s="32"/>
       <c r="J13" s="1">
         <v>41</v>
       </c>
@@ -3256,7 +3515,7 @@
         <v>2599</v>
       </c>
       <c r="L13" s="6"/>
-      <c r="M13" s="11"/>
+      <c r="M13" s="32"/>
       <c r="N13" s="1">
         <v>43</v>
       </c>
@@ -3265,7 +3524,7 @@
       </c>
     </row>
     <row r="14" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="12"/>
+      <c r="A14" s="33"/>
       <c r="B14" s="1">
         <v>45</v>
       </c>
@@ -3273,14 +3532,14 @@
         <v>2601</v>
       </c>
       <c r="D14" s="6"/>
-      <c r="E14" s="10"/>
+      <c r="E14" s="31"/>
       <c r="F14" s="1">
         <v>47</v>
       </c>
       <c r="G14" s="3">
         <v>2472</v>
       </c>
-      <c r="I14" s="9" t="s">
+      <c r="I14" s="30" t="s">
         <v>5</v>
       </c>
       <c r="J14" s="1">
@@ -3290,7 +3549,7 @@
         <v>2368</v>
       </c>
       <c r="L14" s="6"/>
-      <c r="M14" s="9" t="s">
+      <c r="M14" s="30" t="s">
         <v>7</v>
       </c>
       <c r="N14" s="1">
@@ -3301,7 +3560,7 @@
       </c>
     </row>
     <row r="15" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="12"/>
+      <c r="A15" s="33"/>
       <c r="B15" s="1">
         <v>49</v>
       </c>
@@ -3309,14 +3568,14 @@
         <v>2563</v>
       </c>
       <c r="D15" s="6"/>
-      <c r="E15" s="10"/>
+      <c r="E15" s="31"/>
       <c r="F15" s="1">
         <v>51</v>
       </c>
       <c r="G15" s="3">
         <v>2424</v>
       </c>
-      <c r="I15" s="10"/>
+      <c r="I15" s="31"/>
       <c r="J15" s="1">
         <v>6</v>
       </c>
@@ -3324,7 +3583,7 @@
         <v>2382</v>
       </c>
       <c r="L15" s="6"/>
-      <c r="M15" s="10"/>
+      <c r="M15" s="31"/>
       <c r="N15" s="1">
         <v>8</v>
       </c>
@@ -3333,7 +3592,7 @@
       </c>
     </row>
     <row r="16" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="12"/>
+      <c r="A16" s="33"/>
       <c r="B16" s="1">
         <v>53</v>
       </c>
@@ -3341,14 +3600,14 @@
         <v>2613</v>
       </c>
       <c r="D16" s="6"/>
-      <c r="E16" s="10"/>
+      <c r="E16" s="31"/>
       <c r="F16" s="1">
         <v>55</v>
       </c>
       <c r="G16" s="3">
         <v>2469</v>
       </c>
-      <c r="I16" s="10"/>
+      <c r="I16" s="31"/>
       <c r="J16" s="1">
         <v>10</v>
       </c>
@@ -3356,7 +3615,7 @@
         <v>2389</v>
       </c>
       <c r="L16" s="6"/>
-      <c r="M16" s="10"/>
+      <c r="M16" s="31"/>
       <c r="N16" s="1">
         <v>12</v>
       </c>
@@ -3365,7 +3624,7 @@
       </c>
     </row>
     <row r="17" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="12"/>
+      <c r="A17" s="33"/>
       <c r="B17" s="1">
         <v>57</v>
       </c>
@@ -3373,14 +3632,14 @@
         <v>2624</v>
       </c>
       <c r="D17" s="6"/>
-      <c r="E17" s="10"/>
+      <c r="E17" s="31"/>
       <c r="F17" s="1">
         <v>59</v>
       </c>
       <c r="G17" s="3">
         <v>2413</v>
       </c>
-      <c r="I17" s="10"/>
+      <c r="I17" s="31"/>
       <c r="J17" s="1">
         <v>14</v>
       </c>
@@ -3388,7 +3647,7 @@
         <v>2411</v>
       </c>
       <c r="L17" s="6"/>
-      <c r="M17" s="10"/>
+      <c r="M17" s="31"/>
       <c r="N17" s="1">
         <v>16</v>
       </c>
@@ -3397,7 +3656,7 @@
       </c>
     </row>
     <row r="18" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="12"/>
+      <c r="A18" s="33"/>
       <c r="B18" s="1">
         <v>61</v>
       </c>
@@ -3405,14 +3664,14 @@
         <v>2549</v>
       </c>
       <c r="D18" s="6"/>
-      <c r="E18" s="11"/>
+      <c r="E18" s="32"/>
       <c r="F18" s="1">
         <v>63</v>
       </c>
       <c r="G18" s="3">
         <v>2440</v>
       </c>
-      <c r="I18" s="10"/>
+      <c r="I18" s="31"/>
       <c r="J18" s="1">
         <v>18</v>
       </c>
@@ -3420,7 +3679,7 @@
         <v>2406</v>
       </c>
       <c r="L18" s="6"/>
-      <c r="M18" s="10"/>
+      <c r="M18" s="31"/>
       <c r="N18" s="1">
         <v>20</v>
       </c>
@@ -3429,7 +3688,7 @@
       </c>
     </row>
     <row r="19" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="12" t="s">
+      <c r="A19" s="33" t="s">
         <v>5</v>
       </c>
       <c r="B19" s="1">
@@ -3439,7 +3698,7 @@
         <v>2438</v>
       </c>
       <c r="D19" s="6"/>
-      <c r="E19" s="9" t="s">
+      <c r="E19" s="30" t="s">
         <v>7</v>
       </c>
       <c r="F19" s="1">
@@ -3448,7 +3707,7 @@
       <c r="G19" s="3">
         <v>2779</v>
       </c>
-      <c r="I19" s="10"/>
+      <c r="I19" s="31"/>
       <c r="J19" s="1">
         <v>22</v>
       </c>
@@ -3456,7 +3715,7 @@
         <v>2412</v>
       </c>
       <c r="L19" s="6"/>
-      <c r="M19" s="10"/>
+      <c r="M19" s="31"/>
       <c r="N19" s="1">
         <v>24</v>
       </c>
@@ -3465,7 +3724,7 @@
       </c>
     </row>
     <row r="20" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="12"/>
+      <c r="A20" s="33"/>
       <c r="B20" s="1">
         <v>6</v>
       </c>
@@ -3473,14 +3732,14 @@
         <v>2411</v>
       </c>
       <c r="D20" s="6"/>
-      <c r="E20" s="10"/>
+      <c r="E20" s="31"/>
       <c r="F20" s="1">
         <v>8</v>
       </c>
       <c r="G20" s="3">
         <v>2681</v>
       </c>
-      <c r="I20" s="10"/>
+      <c r="I20" s="31"/>
       <c r="J20" s="1">
         <v>26</v>
       </c>
@@ -3488,7 +3747,7 @@
         <v>2386</v>
       </c>
       <c r="L20" s="6"/>
-      <c r="M20" s="10"/>
+      <c r="M20" s="31"/>
       <c r="N20" s="1">
         <v>28</v>
       </c>
@@ -3497,7 +3756,7 @@
       </c>
     </row>
     <row r="21" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="12"/>
+      <c r="A21" s="33"/>
       <c r="B21" s="1">
         <v>10</v>
       </c>
@@ -3505,14 +3764,14 @@
         <v>2384</v>
       </c>
       <c r="D21" s="6"/>
-      <c r="E21" s="10"/>
+      <c r="E21" s="31"/>
       <c r="F21" s="1">
         <v>12</v>
       </c>
       <c r="G21" s="3">
         <v>2667</v>
       </c>
-      <c r="I21" s="10"/>
+      <c r="I21" s="31"/>
       <c r="J21" s="1">
         <v>30</v>
       </c>
@@ -3520,7 +3779,7 @@
         <v>2390</v>
       </c>
       <c r="L21" s="6"/>
-      <c r="M21" s="10"/>
+      <c r="M21" s="31"/>
       <c r="N21" s="1">
         <v>32</v>
       </c>
@@ -3529,7 +3788,7 @@
       </c>
     </row>
     <row r="22" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="12"/>
+      <c r="A22" s="33"/>
       <c r="B22" s="1">
         <v>14</v>
       </c>
@@ -3537,14 +3796,14 @@
         <v>2422</v>
       </c>
       <c r="D22" s="6"/>
-      <c r="E22" s="10"/>
+      <c r="E22" s="31"/>
       <c r="F22" s="1">
         <v>16</v>
       </c>
       <c r="G22" s="3">
         <v>2785</v>
       </c>
-      <c r="I22" s="10"/>
+      <c r="I22" s="31"/>
       <c r="J22" s="1">
         <v>34</v>
       </c>
@@ -3552,7 +3811,7 @@
         <v>2429</v>
       </c>
       <c r="L22" s="6"/>
-      <c r="M22" s="10"/>
+      <c r="M22" s="31"/>
       <c r="N22" s="1">
         <v>36</v>
       </c>
@@ -3561,7 +3820,7 @@
       </c>
     </row>
     <row r="23" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="12"/>
+      <c r="A23" s="33"/>
       <c r="B23" s="1">
         <v>18</v>
       </c>
@@ -3569,14 +3828,14 @@
         <v>2398</v>
       </c>
       <c r="D23" s="6"/>
-      <c r="E23" s="10"/>
+      <c r="E23" s="31"/>
       <c r="F23" s="1">
         <v>20</v>
       </c>
       <c r="G23" s="3">
         <v>2668</v>
       </c>
-      <c r="I23" s="10"/>
+      <c r="I23" s="31"/>
       <c r="J23" s="1">
         <v>38</v>
       </c>
@@ -3584,7 +3843,7 @@
         <v>2399</v>
       </c>
       <c r="L23" s="6"/>
-      <c r="M23" s="10"/>
+      <c r="M23" s="31"/>
       <c r="N23" s="1">
         <v>40</v>
       </c>
@@ -3593,7 +3852,7 @@
       </c>
     </row>
     <row r="24" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="12"/>
+      <c r="A24" s="33"/>
       <c r="B24" s="1">
         <v>22</v>
       </c>
@@ -3601,14 +3860,14 @@
         <v>2421</v>
       </c>
       <c r="D24" s="6"/>
-      <c r="E24" s="10"/>
+      <c r="E24" s="31"/>
       <c r="F24" s="1">
         <v>24</v>
       </c>
       <c r="G24" s="3">
         <v>2711</v>
       </c>
-      <c r="I24" s="11"/>
+      <c r="I24" s="32"/>
       <c r="J24" s="1">
         <v>42</v>
       </c>
@@ -3616,7 +3875,7 @@
         <v>2392</v>
       </c>
       <c r="L24" s="7"/>
-      <c r="M24" s="11"/>
+      <c r="M24" s="32"/>
       <c r="N24" s="1">
         <v>44</v>
       </c>
@@ -3625,7 +3884,7 @@
       </c>
     </row>
     <row r="25" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="12"/>
+      <c r="A25" s="33"/>
       <c r="B25" s="1">
         <v>26</v>
       </c>
@@ -3633,7 +3892,7 @@
         <v>2414</v>
       </c>
       <c r="D25" s="6"/>
-      <c r="E25" s="10"/>
+      <c r="E25" s="31"/>
       <c r="F25" s="1">
         <v>28</v>
       </c>
@@ -3642,7 +3901,7 @@
       </c>
     </row>
     <row r="26" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="12"/>
+      <c r="A26" s="33"/>
       <c r="B26" s="1">
         <v>30</v>
       </c>
@@ -3650,7 +3909,7 @@
         <v>2425</v>
       </c>
       <c r="D26" s="6"/>
-      <c r="E26" s="10"/>
+      <c r="E26" s="31"/>
       <c r="F26" s="1">
         <v>32</v>
       </c>
@@ -3659,7 +3918,7 @@
       </c>
     </row>
     <row r="27" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="12"/>
+      <c r="A27" s="33"/>
       <c r="B27" s="1">
         <v>34</v>
       </c>
@@ -3667,7 +3926,7 @@
         <v>2420</v>
       </c>
       <c r="D27" s="6"/>
-      <c r="E27" s="10"/>
+      <c r="E27" s="31"/>
       <c r="F27" s="1">
         <v>36</v>
       </c>
@@ -3676,7 +3935,7 @@
       </c>
     </row>
     <row r="28" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="12"/>
+      <c r="A28" s="33"/>
       <c r="B28" s="1">
         <v>38</v>
       </c>
@@ -3684,7 +3943,7 @@
         <v>2414</v>
       </c>
       <c r="D28" s="6"/>
-      <c r="E28" s="10"/>
+      <c r="E28" s="31"/>
       <c r="F28" s="1">
         <v>40</v>
       </c>
@@ -3693,7 +3952,7 @@
       </c>
     </row>
     <row r="29" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="12"/>
+      <c r="A29" s="33"/>
       <c r="B29" s="1">
         <v>42</v>
       </c>
@@ -3701,7 +3960,7 @@
         <v>2389</v>
       </c>
       <c r="D29" s="6"/>
-      <c r="E29" s="10"/>
+      <c r="E29" s="31"/>
       <c r="F29" s="1">
         <v>44</v>
       </c>
@@ -3710,7 +3969,7 @@
       </c>
     </row>
     <row r="30" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="12"/>
+      <c r="A30" s="33"/>
       <c r="B30" s="1">
         <v>46</v>
       </c>
@@ -3718,7 +3977,7 @@
         <v>2397</v>
       </c>
       <c r="D30" s="6"/>
-      <c r="E30" s="10"/>
+      <c r="E30" s="31"/>
       <c r="F30" s="1">
         <v>48</v>
       </c>
@@ -3727,7 +3986,7 @@
       </c>
     </row>
     <row r="31" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="12"/>
+      <c r="A31" s="33"/>
       <c r="B31" s="1">
         <v>50</v>
       </c>
@@ -3735,7 +3994,7 @@
         <v>2409</v>
       </c>
       <c r="D31" s="6"/>
-      <c r="E31" s="10"/>
+      <c r="E31" s="31"/>
       <c r="F31" s="1">
         <v>52</v>
       </c>
@@ -3744,7 +4003,7 @@
       </c>
     </row>
     <row r="32" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="12"/>
+      <c r="A32" s="33"/>
       <c r="B32" s="1">
         <v>54</v>
       </c>
@@ -3752,7 +4011,7 @@
         <v>2416</v>
       </c>
       <c r="D32" s="6"/>
-      <c r="E32" s="10"/>
+      <c r="E32" s="31"/>
       <c r="F32" s="1">
         <v>56</v>
       </c>
@@ -3761,7 +4020,7 @@
       </c>
     </row>
     <row r="33" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="12"/>
+      <c r="A33" s="33"/>
       <c r="B33" s="1">
         <v>58</v>
       </c>
@@ -3769,7 +4028,7 @@
         <v>2433</v>
       </c>
       <c r="D33" s="6"/>
-      <c r="E33" s="10"/>
+      <c r="E33" s="31"/>
       <c r="F33" s="1">
         <v>60</v>
       </c>
@@ -3778,7 +4037,7 @@
       </c>
     </row>
     <row r="34" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="12"/>
+      <c r="A34" s="33"/>
       <c r="B34" s="1">
         <v>62</v>
       </c>
@@ -3786,7 +4045,7 @@
         <v>2409</v>
       </c>
       <c r="D34" s="7"/>
-      <c r="E34" s="11"/>
+      <c r="E34" s="32"/>
       <c r="F34" s="1">
         <v>64</v>
       </c>
@@ -3829,10 +4088,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4C523F4-74B3-4E7D-8BAC-552A17169E6B}">
-  <dimension ref="A1:U34"/>
+  <dimension ref="A1:AC34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="S25" sqref="S25"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="X26" sqref="X26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3852,45 +4111,61 @@
     <col min="17" max="17" width="8.6640625" customWidth="1"/>
     <col min="18" max="18" width="8.44140625" customWidth="1"/>
     <col min="19" max="21" width="10.21875" customWidth="1"/>
+    <col min="23" max="23" width="9.6640625" customWidth="1"/>
+    <col min="24" max="24" width="14.88671875" customWidth="1"/>
+    <col min="25" max="25" width="12.33203125" customWidth="1"/>
+    <col min="27" max="27" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="9.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:29" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="I1" s="12" t="s">
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="43"/>
+      <c r="I1" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
-      <c r="M1" s="12"/>
-      <c r="N1" s="12"/>
-      <c r="O1" s="12"/>
-      <c r="Q1" s="21" t="s">
+      <c r="J1" s="42"/>
+      <c r="K1" s="42"/>
+      <c r="L1" s="42"/>
+      <c r="M1" s="42"/>
+      <c r="N1" s="42"/>
+      <c r="O1" s="43"/>
+      <c r="Q1" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="R1" s="22" t="s">
+      <c r="R1" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="S1" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="T1" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="U1" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="S1" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="T1" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="U1" s="24" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:21" ht="18" x14ac:dyDescent="0.35">
-      <c r="A2" s="4" t="s">
+      <c r="W1" s="56" t="s">
+        <v>20</v>
+      </c>
+      <c r="X1" s="57"/>
+      <c r="Y1" s="58"/>
+      <c r="AA1" s="56" t="s">
+        <v>21</v>
+      </c>
+      <c r="AB1" s="57"/>
+      <c r="AC1" s="58"/>
+    </row>
+    <row r="2" spans="1:29" ht="18" x14ac:dyDescent="0.35">
+      <c r="A2" s="44" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -3906,11 +4181,11 @@
       <c r="F2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="45" t="s">
         <v>12</v>
       </c>
       <c r="H2" s="2"/>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="44" t="s">
         <v>8</v>
       </c>
       <c r="J2" s="4" t="s">
@@ -3926,30 +4201,42 @@
       <c r="N2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="O2" s="4" t="s">
+      <c r="O2" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="Q2" s="25">
-        <v>1</v>
-      </c>
-      <c r="R2" s="26" t="s">
+      <c r="Q2" s="34">
+        <v>1</v>
+      </c>
+      <c r="R2" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="S2" s="27">
+      <c r="S2" s="22">
         <f>AVERAGE($C$3:$C$18)</f>
         <v>2587.0625</v>
       </c>
-      <c r="T2" s="28">
+      <c r="T2" s="23">
         <f>_xlfn.STDEV.S($C$3:$C$18)</f>
         <v>29.672588360303184</v>
       </c>
-      <c r="U2" s="29">
+      <c r="U2" s="24">
         <f>COUNT($C$3:$C$18)</f>
         <v>16</v>
       </c>
-    </row>
-    <row r="3" spans="1:21" ht="18" x14ac:dyDescent="0.35">
-      <c r="A3" s="12" t="s">
+      <c r="W2" s="59" t="s">
+        <v>8</v>
+      </c>
+      <c r="X2" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="Y2" s="60" t="s">
+        <v>19</v>
+      </c>
+      <c r="AA2" s="59"/>
+      <c r="AB2" s="9"/>
+      <c r="AC2" s="60"/>
+    </row>
+    <row r="3" spans="1:29" ht="18" x14ac:dyDescent="0.35">
+      <c r="A3" s="54" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="1">
@@ -3959,53 +4246,65 @@
         <v>2565</v>
       </c>
       <c r="D3" s="6"/>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="30" t="s">
         <v>6</v>
       </c>
       <c r="F3" s="1">
         <v>3</v>
       </c>
-      <c r="G3" s="3">
+      <c r="G3" s="47">
         <v>2441</v>
       </c>
-      <c r="I3" s="9" t="s">
+      <c r="I3" s="46" t="s">
         <v>4</v>
       </c>
       <c r="J3" s="1">
         <v>1</v>
       </c>
-      <c r="K3" s="37">
+      <c r="K3" s="29">
         <v>2393</v>
       </c>
       <c r="L3" s="6"/>
-      <c r="M3" s="9" t="s">
+      <c r="M3" s="30" t="s">
         <v>6</v>
       </c>
       <c r="N3" s="1">
         <v>3</v>
       </c>
-      <c r="O3" s="3">
+      <c r="O3" s="47">
         <v>2438</v>
       </c>
-      <c r="Q3" s="17"/>
-      <c r="R3" s="13" t="s">
+      <c r="Q3" s="35"/>
+      <c r="R3" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="S3" s="14">
+      <c r="S3" s="11">
         <f>AVERAGE($C$19:$C$34)</f>
         <v>2412.5</v>
       </c>
-      <c r="T3" s="15">
+      <c r="T3" s="12">
         <f>_xlfn.STDEV.S($C$19:$C$34)</f>
         <v>14.841383583300672</v>
       </c>
-      <c r="U3" s="16">
+      <c r="U3" s="13">
         <f>COUNT($C$19:$C$34)</f>
         <v>16</v>
       </c>
-    </row>
-    <row r="4" spans="1:21" ht="18" x14ac:dyDescent="0.35">
-      <c r="A4" s="12"/>
+      <c r="W3" s="61" t="s">
+        <v>4</v>
+      </c>
+      <c r="X3" s="40">
+        <v>0.96</v>
+      </c>
+      <c r="Y3" s="62">
+        <v>0.39100000000000001</v>
+      </c>
+      <c r="AA3" s="61"/>
+      <c r="AB3" s="40"/>
+      <c r="AC3" s="62"/>
+    </row>
+    <row r="4" spans="1:29" ht="18" x14ac:dyDescent="0.35">
+      <c r="A4" s="54"/>
       <c r="B4" s="1">
         <v>5</v>
       </c>
@@ -4013,14 +4312,14 @@
         <v>2532</v>
       </c>
       <c r="D4" s="6"/>
-      <c r="E4" s="10"/>
+      <c r="E4" s="31"/>
       <c r="F4" s="1">
         <v>7</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G4" s="47">
         <v>2436</v>
       </c>
-      <c r="I4" s="10"/>
+      <c r="I4" s="35"/>
       <c r="J4" s="1">
         <v>5</v>
       </c>
@@ -4028,32 +4327,44 @@
         <v>2550</v>
       </c>
       <c r="L4" s="6"/>
-      <c r="M4" s="10"/>
+      <c r="M4" s="31"/>
       <c r="N4" s="1">
         <v>7</v>
       </c>
-      <c r="O4" s="3">
+      <c r="O4" s="47">
         <v>2439</v>
       </c>
-      <c r="Q4" s="17"/>
-      <c r="R4" s="13" t="s">
+      <c r="Q4" s="35"/>
+      <c r="R4" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="S4" s="14">
+      <c r="S4" s="11">
         <f>AVERAGE($G$3:$G$18)</f>
         <v>2437.4375</v>
       </c>
-      <c r="T4" s="15">
+      <c r="T4" s="12">
         <f>_xlfn.STDEV.S($G$3:$G$18)</f>
         <v>19.599213419590765</v>
       </c>
-      <c r="U4" s="16">
+      <c r="U4" s="13">
         <f>COUNT($G$3:$G$18)</f>
         <v>16</v>
       </c>
-    </row>
-    <row r="5" spans="1:21" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="12"/>
+      <c r="W4" s="61" t="s">
+        <v>5</v>
+      </c>
+      <c r="X4" s="39">
+        <v>0.97940000000000005</v>
+      </c>
+      <c r="Y4" s="62">
+        <v>0.84899999999999998</v>
+      </c>
+      <c r="AA4" s="61"/>
+      <c r="AB4" s="39"/>
+      <c r="AC4" s="62"/>
+    </row>
+    <row r="5" spans="1:29" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="54"/>
       <c r="B5" s="1">
         <v>9</v>
       </c>
@@ -4061,14 +4372,14 @@
         <v>2566</v>
       </c>
       <c r="D5" s="6"/>
-      <c r="E5" s="10"/>
+      <c r="E5" s="31"/>
       <c r="F5" s="1">
         <v>11</v>
       </c>
-      <c r="G5" s="3">
+      <c r="G5" s="47">
         <v>2441</v>
       </c>
-      <c r="I5" s="10"/>
+      <c r="I5" s="35"/>
       <c r="J5" s="1">
         <v>9</v>
       </c>
@@ -4076,32 +4387,44 @@
         <v>2599</v>
       </c>
       <c r="L5" s="6"/>
-      <c r="M5" s="10"/>
+      <c r="M5" s="31"/>
       <c r="N5" s="1">
         <v>11</v>
       </c>
-      <c r="O5" s="3">
+      <c r="O5" s="47">
         <v>2460</v>
       </c>
-      <c r="Q5" s="30"/>
-      <c r="R5" s="31" t="s">
+      <c r="Q5" s="36"/>
+      <c r="R5" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="S5" s="18">
+      <c r="S5" s="14">
         <f>AVERAGE($G$19:$G$34)</f>
         <v>2731.5625</v>
       </c>
-      <c r="T5" s="19">
+      <c r="T5" s="15">
         <f>_xlfn.STDEV.S($G$19:$G$34)</f>
         <v>43.335849285935694</v>
       </c>
-      <c r="U5" s="20">
+      <c r="U5" s="16">
         <f>COUNT($G$19:$G$34)</f>
         <v>16</v>
       </c>
-    </row>
-    <row r="6" spans="1:21" ht="18" x14ac:dyDescent="0.35">
-      <c r="A6" s="12"/>
+      <c r="W5" s="61" t="s">
+        <v>6</v>
+      </c>
+      <c r="X5" s="39">
+        <v>0.97860000000000003</v>
+      </c>
+      <c r="Y5" s="62">
+        <v>0.82899999999999996</v>
+      </c>
+      <c r="AA5" s="61"/>
+      <c r="AB5" s="39"/>
+      <c r="AC5" s="62"/>
+    </row>
+    <row r="6" spans="1:29" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="54"/>
       <c r="B6" s="1">
         <v>13</v>
       </c>
@@ -4109,14 +4432,14 @@
         <v>2586</v>
       </c>
       <c r="D6" s="6"/>
-      <c r="E6" s="10"/>
+      <c r="E6" s="31"/>
       <c r="F6" s="1">
         <v>15</v>
       </c>
-      <c r="G6" s="3">
+      <c r="G6" s="47">
         <v>2438</v>
       </c>
-      <c r="I6" s="10"/>
+      <c r="I6" s="35"/>
       <c r="J6" s="1">
         <v>13</v>
       </c>
@@ -4124,34 +4447,46 @@
         <v>2583</v>
       </c>
       <c r="L6" s="6"/>
-      <c r="M6" s="10"/>
+      <c r="M6" s="31"/>
       <c r="N6" s="1">
         <v>15</v>
       </c>
-      <c r="O6" s="3">
+      <c r="O6" s="47">
         <v>2415</v>
       </c>
-      <c r="Q6" s="25">
+      <c r="Q6" s="34">
         <v>2</v>
       </c>
-      <c r="R6" s="26" t="s">
+      <c r="R6" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="S6" s="27">
+      <c r="S6" s="22">
         <f>AVERAGE($K$4:$K$13)</f>
         <v>2582.1999999999998</v>
       </c>
-      <c r="T6" s="28">
+      <c r="T6" s="23">
         <f>_xlfn.STDEV.S($K$4:$K$13)</f>
         <v>23.102669398433882</v>
       </c>
-      <c r="U6" s="29">
+      <c r="U6" s="24">
         <f>COUNT($K$4:$K$13)</f>
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:21" ht="18" x14ac:dyDescent="0.35">
-      <c r="A7" s="12"/>
+      <c r="W6" s="63" t="s">
+        <v>7</v>
+      </c>
+      <c r="X6" s="64">
+        <v>0.96430000000000005</v>
+      </c>
+      <c r="Y6" s="65">
+        <v>0.45900000000000002</v>
+      </c>
+      <c r="AA6" s="63"/>
+      <c r="AB6" s="64"/>
+      <c r="AC6" s="65"/>
+    </row>
+    <row r="7" spans="1:29" ht="18" x14ac:dyDescent="0.35">
+      <c r="A7" s="54"/>
       <c r="B7" s="1">
         <v>17</v>
       </c>
@@ -4159,14 +4494,14 @@
         <v>2613</v>
       </c>
       <c r="D7" s="6"/>
-      <c r="E7" s="10"/>
+      <c r="E7" s="31"/>
       <c r="F7" s="1">
         <v>19</v>
       </c>
-      <c r="G7" s="3">
+      <c r="G7" s="47">
         <v>2425</v>
       </c>
-      <c r="I7" s="10"/>
+      <c r="I7" s="35"/>
       <c r="J7" s="1">
         <v>17</v>
       </c>
@@ -4174,32 +4509,32 @@
         <v>2604</v>
       </c>
       <c r="L7" s="6"/>
-      <c r="M7" s="10"/>
+      <c r="M7" s="31"/>
       <c r="N7" s="1">
         <v>19</v>
       </c>
-      <c r="O7" s="3">
+      <c r="O7" s="47">
         <v>2419</v>
       </c>
-      <c r="Q7" s="17"/>
-      <c r="R7" s="13" t="s">
+      <c r="Q7" s="35"/>
+      <c r="R7" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="S7" s="14">
+      <c r="S7" s="11">
         <f>AVERAGE($K$14:$K$24)</f>
         <v>2396.7272727272725</v>
       </c>
-      <c r="T7" s="15">
+      <c r="T7" s="12">
         <f>_xlfn.STDEV.S($K$14:$K$24)</f>
         <v>16.894323952682505</v>
       </c>
-      <c r="U7" s="16">
+      <c r="U7" s="13">
         <f>COUNT($K$14:$K$24)</f>
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:21" ht="18" x14ac:dyDescent="0.35">
-      <c r="A8" s="12"/>
+    <row r="8" spans="1:29" ht="18" x14ac:dyDescent="0.35">
+      <c r="A8" s="54"/>
       <c r="B8" s="1">
         <v>21</v>
       </c>
@@ -4207,14 +4542,14 @@
         <v>2621</v>
       </c>
       <c r="D8" s="6"/>
-      <c r="E8" s="10"/>
+      <c r="E8" s="31"/>
       <c r="F8" s="1">
         <v>23</v>
       </c>
-      <c r="G8" s="3">
+      <c r="G8" s="47">
         <v>2429</v>
       </c>
-      <c r="I8" s="10"/>
+      <c r="I8" s="35"/>
       <c r="J8" s="1">
         <v>21</v>
       </c>
@@ -4222,32 +4557,32 @@
         <v>2566</v>
       </c>
       <c r="L8" s="6"/>
-      <c r="M8" s="10"/>
+      <c r="M8" s="31"/>
       <c r="N8" s="1">
         <v>23</v>
       </c>
-      <c r="O8" s="3">
+      <c r="O8" s="47">
         <v>2446</v>
       </c>
-      <c r="Q8" s="17"/>
-      <c r="R8" s="13" t="s">
+      <c r="Q8" s="35"/>
+      <c r="R8" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="S8" s="14">
+      <c r="S8" s="11">
         <f>AVERAGE($O$3:$O$13)</f>
         <v>2428.818181818182</v>
       </c>
-      <c r="T8" s="15">
+      <c r="T8" s="12">
         <f>_xlfn.STDEV.S($O$3:$O$13)</f>
         <v>17.769739344279539</v>
       </c>
-      <c r="U8" s="16">
+      <c r="U8" s="13">
         <f>COUNT($O$3:$O$13)</f>
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:21" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="12"/>
+    <row r="9" spans="1:29" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="54"/>
       <c r="B9" s="1">
         <v>25</v>
       </c>
@@ -4255,14 +4590,14 @@
         <v>2608</v>
       </c>
       <c r="D9" s="6"/>
-      <c r="E9" s="10"/>
+      <c r="E9" s="31"/>
       <c r="F9" s="1">
         <v>27</v>
       </c>
-      <c r="G9" s="3">
+      <c r="G9" s="47">
         <v>2410</v>
       </c>
-      <c r="I9" s="10"/>
+      <c r="I9" s="35"/>
       <c r="J9" s="1">
         <v>25</v>
       </c>
@@ -4270,32 +4605,32 @@
         <v>2582</v>
       </c>
       <c r="L9" s="6"/>
-      <c r="M9" s="10"/>
+      <c r="M9" s="31"/>
       <c r="N9" s="1">
         <v>27</v>
       </c>
-      <c r="O9" s="3">
+      <c r="O9" s="47">
         <v>2438</v>
       </c>
-      <c r="Q9" s="30"/>
-      <c r="R9" s="31" t="s">
+      <c r="Q9" s="36"/>
+      <c r="R9" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="S9" s="18">
+      <c r="S9" s="14">
         <f>AVERAGE($O$14:$O$24)</f>
         <v>2719.6363636363635</v>
       </c>
-      <c r="T9" s="19">
+      <c r="T9" s="15">
         <f>_xlfn.STDEV.S($O$14:$O$24)</f>
         <v>33.317481079075371</v>
       </c>
-      <c r="U9" s="20">
+      <c r="U9" s="16">
         <f>COUNT($O$14:$O$24)</f>
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:21" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="12"/>
+    <row r="10" spans="1:29" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="54"/>
       <c r="B10" s="1">
         <v>29</v>
       </c>
@@ -4303,14 +4638,14 @@
         <v>2631</v>
       </c>
       <c r="D10" s="6"/>
-      <c r="E10" s="10"/>
+      <c r="E10" s="31"/>
       <c r="F10" s="1">
         <v>31</v>
       </c>
-      <c r="G10" s="3">
+      <c r="G10" s="47">
         <v>2462</v>
       </c>
-      <c r="I10" s="10"/>
+      <c r="I10" s="35"/>
       <c r="J10" s="1">
         <v>29</v>
       </c>
@@ -4318,32 +4653,32 @@
         <v>2558</v>
       </c>
       <c r="L10" s="6"/>
-      <c r="M10" s="10"/>
+      <c r="M10" s="31"/>
       <c r="N10" s="1">
         <v>31</v>
       </c>
-      <c r="O10" s="3">
+      <c r="O10" s="47">
         <v>2394</v>
       </c>
-      <c r="Q10" s="32" t="s">
-        <v>18</v>
-      </c>
-      <c r="R10" s="33"/>
-      <c r="S10" s="34">
+      <c r="Q10" s="37" t="s">
+        <v>17</v>
+      </c>
+      <c r="R10" s="38"/>
+      <c r="S10" s="26">
         <f>AVERAGE(S2:S9)</f>
         <v>2536.9930397727271</v>
       </c>
-      <c r="T10" s="35">
+      <c r="T10" s="27">
         <f>_xlfn.STDEV.S($C$3:$C$34,$G$3:$G$34,$K$3:$K$24,$O$3:$O$24)</f>
         <v>132.47919662702068</v>
       </c>
-      <c r="U10" s="36">
+      <c r="U10" s="28">
         <f>SUM(U2:U9)</f>
         <v>107</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A11" s="12"/>
+    <row r="11" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A11" s="54"/>
       <c r="B11" s="1">
         <v>33</v>
       </c>
@@ -4351,14 +4686,14 @@
         <v>2564</v>
       </c>
       <c r="D11" s="6"/>
-      <c r="E11" s="10"/>
+      <c r="E11" s="31"/>
       <c r="F11" s="1">
         <v>35</v>
       </c>
-      <c r="G11" s="3">
+      <c r="G11" s="47">
         <v>2443</v>
       </c>
-      <c r="I11" s="10"/>
+      <c r="I11" s="35"/>
       <c r="J11" s="1">
         <v>33</v>
       </c>
@@ -4366,16 +4701,16 @@
         <v>2561</v>
       </c>
       <c r="L11" s="6"/>
-      <c r="M11" s="10"/>
+      <c r="M11" s="31"/>
       <c r="N11" s="1">
         <v>35</v>
       </c>
-      <c r="O11" s="3">
+      <c r="O11" s="47">
         <v>2423</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A12" s="12"/>
+    <row r="12" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A12" s="54"/>
       <c r="B12" s="1">
         <v>37</v>
       </c>
@@ -4383,14 +4718,14 @@
         <v>2571</v>
       </c>
       <c r="D12" s="6"/>
-      <c r="E12" s="10"/>
+      <c r="E12" s="31"/>
       <c r="F12" s="1">
         <v>39</v>
       </c>
-      <c r="G12" s="3">
+      <c r="G12" s="47">
         <v>2450</v>
       </c>
-      <c r="I12" s="10"/>
+      <c r="I12" s="35"/>
       <c r="J12" s="1">
         <v>37</v>
       </c>
@@ -4398,16 +4733,16 @@
         <v>2620</v>
       </c>
       <c r="L12" s="6"/>
-      <c r="M12" s="10"/>
+      <c r="M12" s="31"/>
       <c r="N12" s="1">
         <v>39</v>
       </c>
-      <c r="O12" s="3">
+      <c r="O12" s="47">
         <v>2424</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A13" s="12"/>
+    <row r="13" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A13" s="54"/>
       <c r="B13" s="1">
         <v>41</v>
       </c>
@@ -4415,14 +4750,14 @@
         <v>2586</v>
       </c>
       <c r="D13" s="6"/>
-      <c r="E13" s="10"/>
+      <c r="E13" s="31"/>
       <c r="F13" s="1">
         <v>43</v>
       </c>
-      <c r="G13" s="3">
+      <c r="G13" s="47">
         <v>2406</v>
       </c>
-      <c r="I13" s="11"/>
+      <c r="I13" s="48"/>
       <c r="J13" s="1">
         <v>41</v>
       </c>
@@ -4430,16 +4765,16 @@
         <v>2599</v>
       </c>
       <c r="L13" s="6"/>
-      <c r="M13" s="11"/>
+      <c r="M13" s="32"/>
       <c r="N13" s="1">
         <v>43</v>
       </c>
-      <c r="O13" s="3">
+      <c r="O13" s="47">
         <v>2421</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A14" s="12"/>
+    <row r="14" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A14" s="54"/>
       <c r="B14" s="1">
         <v>45</v>
       </c>
@@ -4447,14 +4782,14 @@
         <v>2601</v>
       </c>
       <c r="D14" s="6"/>
-      <c r="E14" s="10"/>
+      <c r="E14" s="31"/>
       <c r="F14" s="1">
         <v>47</v>
       </c>
-      <c r="G14" s="3">
+      <c r="G14" s="47">
         <v>2472</v>
       </c>
-      <c r="I14" s="9" t="s">
+      <c r="I14" s="46" t="s">
         <v>5</v>
       </c>
       <c r="J14" s="1">
@@ -4464,18 +4799,18 @@
         <v>2368</v>
       </c>
       <c r="L14" s="6"/>
-      <c r="M14" s="9" t="s">
+      <c r="M14" s="30" t="s">
         <v>7</v>
       </c>
       <c r="N14" s="1">
         <v>4</v>
       </c>
-      <c r="O14" s="3">
+      <c r="O14" s="47">
         <v>2753</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A15" s="12"/>
+    <row r="15" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A15" s="54"/>
       <c r="B15" s="1">
         <v>49</v>
       </c>
@@ -4483,14 +4818,14 @@
         <v>2563</v>
       </c>
       <c r="D15" s="6"/>
-      <c r="E15" s="10"/>
+      <c r="E15" s="31"/>
       <c r="F15" s="1">
         <v>51</v>
       </c>
-      <c r="G15" s="3">
+      <c r="G15" s="47">
         <v>2424</v>
       </c>
-      <c r="I15" s="10"/>
+      <c r="I15" s="35"/>
       <c r="J15" s="1">
         <v>6</v>
       </c>
@@ -4498,16 +4833,16 @@
         <v>2382</v>
       </c>
       <c r="L15" s="6"/>
-      <c r="M15" s="10"/>
+      <c r="M15" s="31"/>
       <c r="N15" s="1">
         <v>8</v>
       </c>
-      <c r="O15" s="3">
+      <c r="O15" s="47">
         <v>2688</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A16" s="12"/>
+    <row r="16" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A16" s="54"/>
       <c r="B16" s="1">
         <v>53</v>
       </c>
@@ -4515,14 +4850,14 @@
         <v>2613</v>
       </c>
       <c r="D16" s="6"/>
-      <c r="E16" s="10"/>
+      <c r="E16" s="31"/>
       <c r="F16" s="1">
         <v>55</v>
       </c>
-      <c r="G16" s="3">
+      <c r="G16" s="47">
         <v>2469</v>
       </c>
-      <c r="I16" s="10"/>
+      <c r="I16" s="35"/>
       <c r="J16" s="1">
         <v>10</v>
       </c>
@@ -4530,16 +4865,16 @@
         <v>2389</v>
       </c>
       <c r="L16" s="6"/>
-      <c r="M16" s="10"/>
+      <c r="M16" s="31"/>
       <c r="N16" s="1">
         <v>12</v>
       </c>
-      <c r="O16" s="3">
+      <c r="O16" s="47">
         <v>2773</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A17" s="12"/>
+      <c r="A17" s="54"/>
       <c r="B17" s="1">
         <v>57</v>
       </c>
@@ -4547,14 +4882,14 @@
         <v>2624</v>
       </c>
       <c r="D17" s="6"/>
-      <c r="E17" s="10"/>
+      <c r="E17" s="31"/>
       <c r="F17" s="1">
         <v>59</v>
       </c>
-      <c r="G17" s="3">
+      <c r="G17" s="47">
         <v>2413</v>
       </c>
-      <c r="I17" s="10"/>
+      <c r="I17" s="35"/>
       <c r="J17" s="1">
         <v>14</v>
       </c>
@@ -4562,16 +4897,16 @@
         <v>2411</v>
       </c>
       <c r="L17" s="6"/>
-      <c r="M17" s="10"/>
+      <c r="M17" s="31"/>
       <c r="N17" s="1">
         <v>16</v>
       </c>
-      <c r="O17" s="3">
+      <c r="O17" s="47">
         <v>2741</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A18" s="12"/>
+      <c r="A18" s="54"/>
       <c r="B18" s="1">
         <v>61</v>
       </c>
@@ -4579,14 +4914,14 @@
         <v>2549</v>
       </c>
       <c r="D18" s="6"/>
-      <c r="E18" s="11"/>
+      <c r="E18" s="32"/>
       <c r="F18" s="1">
         <v>63</v>
       </c>
-      <c r="G18" s="3">
+      <c r="G18" s="47">
         <v>2440</v>
       </c>
-      <c r="I18" s="10"/>
+      <c r="I18" s="35"/>
       <c r="J18" s="1">
         <v>18</v>
       </c>
@@ -4594,16 +4929,16 @@
         <v>2406</v>
       </c>
       <c r="L18" s="6"/>
-      <c r="M18" s="10"/>
+      <c r="M18" s="31"/>
       <c r="N18" s="1">
         <v>20</v>
       </c>
-      <c r="O18" s="3">
+      <c r="O18" s="47">
         <v>2692</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A19" s="12" t="s">
+      <c r="A19" s="54" t="s">
         <v>5</v>
       </c>
       <c r="B19" s="1">
@@ -4613,16 +4948,16 @@
         <v>2438</v>
       </c>
       <c r="D19" s="6"/>
-      <c r="E19" s="9" t="s">
+      <c r="E19" s="30" t="s">
         <v>7</v>
       </c>
       <c r="F19" s="1">
         <v>4</v>
       </c>
-      <c r="G19" s="3">
+      <c r="G19" s="47">
         <v>2779</v>
       </c>
-      <c r="I19" s="10"/>
+      <c r="I19" s="35"/>
       <c r="J19" s="1">
         <v>22</v>
       </c>
@@ -4630,16 +4965,16 @@
         <v>2412</v>
       </c>
       <c r="L19" s="6"/>
-      <c r="M19" s="10"/>
+      <c r="M19" s="31"/>
       <c r="N19" s="1">
         <v>24</v>
       </c>
-      <c r="O19" s="3">
+      <c r="O19" s="47">
         <v>2740</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A20" s="12"/>
+      <c r="A20" s="54"/>
       <c r="B20" s="1">
         <v>6</v>
       </c>
@@ -4647,14 +4982,14 @@
         <v>2411</v>
       </c>
       <c r="D20" s="6"/>
-      <c r="E20" s="10"/>
+      <c r="E20" s="31"/>
       <c r="F20" s="1">
         <v>8</v>
       </c>
-      <c r="G20" s="3">
+      <c r="G20" s="47">
         <v>2681</v>
       </c>
-      <c r="I20" s="10"/>
+      <c r="I20" s="35"/>
       <c r="J20" s="1">
         <v>26</v>
       </c>
@@ -4662,16 +4997,16 @@
         <v>2386</v>
       </c>
       <c r="L20" s="6"/>
-      <c r="M20" s="10"/>
+      <c r="M20" s="31"/>
       <c r="N20" s="1">
         <v>28</v>
       </c>
-      <c r="O20" s="3">
+      <c r="O20" s="47">
         <v>2737</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A21" s="12"/>
+      <c r="A21" s="54"/>
       <c r="B21" s="1">
         <v>10</v>
       </c>
@@ -4679,14 +5014,14 @@
         <v>2384</v>
       </c>
       <c r="D21" s="6"/>
-      <c r="E21" s="10"/>
+      <c r="E21" s="31"/>
       <c r="F21" s="1">
         <v>12</v>
       </c>
-      <c r="G21" s="3">
+      <c r="G21" s="47">
         <v>2667</v>
       </c>
-      <c r="I21" s="10"/>
+      <c r="I21" s="35"/>
       <c r="J21" s="1">
         <v>30</v>
       </c>
@@ -4694,16 +5029,16 @@
         <v>2390</v>
       </c>
       <c r="L21" s="6"/>
-      <c r="M21" s="10"/>
+      <c r="M21" s="31"/>
       <c r="N21" s="1">
         <v>32</v>
       </c>
-      <c r="O21" s="3">
+      <c r="O21" s="47">
         <v>2676</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A22" s="12"/>
+      <c r="A22" s="54"/>
       <c r="B22" s="1">
         <v>14</v>
       </c>
@@ -4711,14 +5046,14 @@
         <v>2422</v>
       </c>
       <c r="D22" s="6"/>
-      <c r="E22" s="10"/>
+      <c r="E22" s="31"/>
       <c r="F22" s="1">
         <v>16</v>
       </c>
-      <c r="G22" s="3">
+      <c r="G22" s="47">
         <v>2785</v>
       </c>
-      <c r="I22" s="10"/>
+      <c r="I22" s="35"/>
       <c r="J22" s="1">
         <v>34</v>
       </c>
@@ -4726,16 +5061,16 @@
         <v>2429</v>
       </c>
       <c r="L22" s="6"/>
-      <c r="M22" s="10"/>
+      <c r="M22" s="31"/>
       <c r="N22" s="1">
         <v>36</v>
       </c>
-      <c r="O22" s="3">
+      <c r="O22" s="47">
         <v>2725</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A23" s="12"/>
+      <c r="A23" s="54"/>
       <c r="B23" s="1">
         <v>18</v>
       </c>
@@ -4743,14 +5078,14 @@
         <v>2398</v>
       </c>
       <c r="D23" s="6"/>
-      <c r="E23" s="10"/>
+      <c r="E23" s="31"/>
       <c r="F23" s="1">
         <v>20</v>
       </c>
-      <c r="G23" s="3">
+      <c r="G23" s="47">
         <v>2668</v>
       </c>
-      <c r="I23" s="10"/>
+      <c r="I23" s="35"/>
       <c r="J23" s="1">
         <v>38</v>
       </c>
@@ -4758,16 +5093,16 @@
         <v>2399</v>
       </c>
       <c r="L23" s="6"/>
-      <c r="M23" s="10"/>
+      <c r="M23" s="31"/>
       <c r="N23" s="1">
         <v>40</v>
       </c>
-      <c r="O23" s="3">
+      <c r="O23" s="47">
         <v>2719</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A24" s="12"/>
+    <row r="24" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="54"/>
       <c r="B24" s="1">
         <v>22</v>
       </c>
@@ -4775,31 +5110,31 @@
         <v>2421</v>
       </c>
       <c r="D24" s="6"/>
-      <c r="E24" s="10"/>
+      <c r="E24" s="31"/>
       <c r="F24" s="1">
         <v>24</v>
       </c>
-      <c r="G24" s="3">
+      <c r="G24" s="47">
         <v>2711</v>
       </c>
-      <c r="I24" s="11"/>
-      <c r="J24" s="1">
+      <c r="I24" s="36"/>
+      <c r="J24" s="49">
         <v>42</v>
       </c>
-      <c r="K24" s="3">
+      <c r="K24" s="50">
         <v>2392</v>
       </c>
-      <c r="L24" s="7"/>
-      <c r="M24" s="11"/>
-      <c r="N24" s="1">
+      <c r="L24" s="51"/>
+      <c r="M24" s="52"/>
+      <c r="N24" s="49">
         <v>44</v>
       </c>
-      <c r="O24" s="3">
+      <c r="O24" s="53">
         <v>2672</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A25" s="12"/>
+      <c r="A25" s="54"/>
       <c r="B25" s="1">
         <v>26</v>
       </c>
@@ -4807,16 +5142,16 @@
         <v>2414</v>
       </c>
       <c r="D25" s="6"/>
-      <c r="E25" s="10"/>
+      <c r="E25" s="31"/>
       <c r="F25" s="1">
         <v>28</v>
       </c>
-      <c r="G25" s="3">
+      <c r="G25" s="47">
         <v>2794</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A26" s="12"/>
+      <c r="A26" s="54"/>
       <c r="B26" s="1">
         <v>30</v>
       </c>
@@ -4824,16 +5159,16 @@
         <v>2425</v>
       </c>
       <c r="D26" s="6"/>
-      <c r="E26" s="10"/>
+      <c r="E26" s="31"/>
       <c r="F26" s="1">
         <v>32</v>
       </c>
-      <c r="G26" s="3">
+      <c r="G26" s="47">
         <v>2712</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A27" s="12"/>
+      <c r="A27" s="54"/>
       <c r="B27" s="1">
         <v>34</v>
       </c>
@@ -4841,16 +5176,16 @@
         <v>2420</v>
       </c>
       <c r="D27" s="6"/>
-      <c r="E27" s="10"/>
+      <c r="E27" s="31"/>
       <c r="F27" s="1">
         <v>36</v>
       </c>
-      <c r="G27" s="3">
+      <c r="G27" s="47">
         <v>2741</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A28" s="12"/>
+      <c r="A28" s="54"/>
       <c r="B28" s="1">
         <v>38</v>
       </c>
@@ -4858,16 +5193,16 @@
         <v>2414</v>
       </c>
       <c r="D28" s="6"/>
-      <c r="E28" s="10"/>
+      <c r="E28" s="31"/>
       <c r="F28" s="1">
         <v>40</v>
       </c>
-      <c r="G28" s="3">
+      <c r="G28" s="47">
         <v>2804</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A29" s="12"/>
+      <c r="A29" s="54"/>
       <c r="B29" s="1">
         <v>42</v>
       </c>
@@ -4875,16 +5210,16 @@
         <v>2389</v>
       </c>
       <c r="D29" s="6"/>
-      <c r="E29" s="10"/>
+      <c r="E29" s="31"/>
       <c r="F29" s="1">
         <v>44</v>
       </c>
-      <c r="G29" s="3">
+      <c r="G29" s="47">
         <v>2727</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A30" s="12"/>
+      <c r="A30" s="54"/>
       <c r="B30" s="1">
         <v>46</v>
       </c>
@@ -4892,16 +5227,16 @@
         <v>2397</v>
       </c>
       <c r="D30" s="6"/>
-      <c r="E30" s="10"/>
+      <c r="E30" s="31"/>
       <c r="F30" s="1">
         <v>48</v>
       </c>
-      <c r="G30" s="3">
+      <c r="G30" s="47">
         <v>2722</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A31" s="12"/>
+      <c r="A31" s="54"/>
       <c r="B31" s="1">
         <v>50</v>
       </c>
@@ -4909,16 +5244,16 @@
         <v>2409</v>
       </c>
       <c r="D31" s="6"/>
-      <c r="E31" s="10"/>
+      <c r="E31" s="31"/>
       <c r="F31" s="1">
         <v>52</v>
       </c>
-      <c r="G31" s="3">
+      <c r="G31" s="47">
         <v>2710</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A32" s="12"/>
+      <c r="A32" s="54"/>
       <c r="B32" s="1">
         <v>54</v>
       </c>
@@ -4926,16 +5261,16 @@
         <v>2416</v>
       </c>
       <c r="D32" s="6"/>
-      <c r="E32" s="10"/>
+      <c r="E32" s="31"/>
       <c r="F32" s="1">
         <v>56</v>
       </c>
-      <c r="G32" s="3">
+      <c r="G32" s="47">
         <v>2739</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33" s="12"/>
+      <c r="A33" s="54"/>
       <c r="B33" s="1">
         <v>58</v>
       </c>
@@ -4943,33 +5278,35 @@
         <v>2433</v>
       </c>
       <c r="D33" s="6"/>
-      <c r="E33" s="10"/>
+      <c r="E33" s="31"/>
       <c r="F33" s="1">
         <v>60</v>
       </c>
-      <c r="G33" s="3">
+      <c r="G33" s="47">
         <v>2704</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A34" s="12"/>
-      <c r="B34" s="1">
+    <row r="34" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="55"/>
+      <c r="B34" s="49">
         <v>62</v>
       </c>
-      <c r="C34" s="3">
+      <c r="C34" s="50">
         <v>2409</v>
       </c>
-      <c r="D34" s="7"/>
-      <c r="E34" s="11"/>
-      <c r="F34" s="1">
+      <c r="D34" s="51"/>
+      <c r="E34" s="52"/>
+      <c r="F34" s="49">
         <v>64</v>
       </c>
-      <c r="G34" s="3">
+      <c r="G34" s="53">
         <v>2761</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="15">
+    <mergeCell ref="W1:Y1"/>
+    <mergeCell ref="AA1:AC1"/>
     <mergeCell ref="Q2:Q5"/>
     <mergeCell ref="Q6:Q9"/>
     <mergeCell ref="Q10:R10"/>
@@ -4986,5 +5323,6 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>